<commit_message>
revising according to Ben Tully's advice
</commit_message>
<xml_diff>
--- a/Figure Generating/data/DNA_Location_Metadata.xlsx
+++ b/Figure Generating/data/DNA_Location_Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Juntao\Desktop\Figure Generating\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Juntao\Desktop\transposase-deep-ocean\Figure Generating\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6A7A90-0EFB-41DF-9CD9-9A5EA1CF0F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D84279-F56E-4B29-A0BC-A112AF6D9841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="205">
   <si>
     <t>TARA_A100000164</t>
   </si>
@@ -646,13 +646,19 @@
   </si>
   <si>
     <t>Ocean_DNA</t>
+  </si>
+  <si>
+    <t>PANGAEA sample id</t>
+  </si>
+  <si>
+    <t>Raw reads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,6 +688,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -705,13 +719,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I304"/>
+  <dimension ref="A1:K304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1005,9 +1020,11 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6">
+    <row r="1" spans="1:11" ht="15.6">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -1035,8 +1052,14 @@
       <c r="I1" s="3" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.6">
+      <c r="J1" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,8 +1088,14 @@
       <c r="I2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.6">
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>415570856</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1095,8 +1124,14 @@
       <c r="I3" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.6">
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>367820654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1125,8 +1160,14 @@
       <c r="I4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.6">
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>488612256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1155,8 +1196,14 @@
       <c r="I5" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.6">
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>398181184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1185,8 +1232,14 @@
       <c r="I6" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.6">
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>394451818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1215,8 +1268,14 @@
       <c r="I7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.6">
+      <c r="J7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>255740402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1245,8 +1304,14 @@
       <c r="I8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.6">
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>403538306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.6">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1272,8 +1337,14 @@
       <c r="I9" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.6">
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <v>221166612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.6">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1299,8 +1370,14 @@
       <c r="I10" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.6">
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>178519830</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.6">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1329,8 +1406,14 @@
       <c r="I11" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.6">
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>291527114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1359,8 +1442,14 @@
       <c r="I12" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.6">
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <v>436200002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.6">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1389,8 +1478,14 @@
       <c r="I13" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.6">
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13">
+        <v>447472502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.6">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1419,8 +1514,14 @@
       <c r="I14" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.6">
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14">
+        <v>323328644</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.6">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1449,8 +1550,14 @@
       <c r="I15" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.6">
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>151854660</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.6">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1476,8 +1583,14 @@
       <c r="I16" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.6">
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16">
+        <v>291429494</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.6">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1506,8 +1619,14 @@
       <c r="I17" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.6">
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17">
+        <v>337711862</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.6">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1536,8 +1655,14 @@
       <c r="I18" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.6">
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18">
+        <v>336385740</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.6">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1566,8 +1691,14 @@
       <c r="I19" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.6">
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <v>324775688</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.6">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1596,8 +1727,14 @@
       <c r="I20" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.6">
+      <c r="J20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20">
+        <v>241970908</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.6">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1626,8 +1763,14 @@
       <c r="I21" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.6">
+      <c r="J21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21">
+        <v>450135214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.6">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1656,8 +1799,14 @@
       <c r="I22" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.6">
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22">
+        <v>402672664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.6">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1686,8 +1835,14 @@
       <c r="I23" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.6">
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23">
+        <v>420102752</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.6">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1716,8 +1871,14 @@
       <c r="I24" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.6">
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>338044892</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.6">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1746,8 +1907,14 @@
       <c r="I25" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.6">
+      <c r="J25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25">
+        <v>402211598</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.6">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1776,8 +1943,14 @@
       <c r="I26" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.6">
+      <c r="J26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26">
+        <v>430413408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.6">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1806,8 +1979,14 @@
       <c r="I27" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.6">
+      <c r="J27" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27">
+        <v>391430950</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.6">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1836,8 +2015,14 @@
       <c r="I28" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.6">
+      <c r="J28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28">
+        <v>404906778</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.6">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1866,8 +2051,14 @@
       <c r="I29" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.6">
+      <c r="J29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29">
+        <v>389259730</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.6">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1896,8 +2087,14 @@
       <c r="I30" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.6">
+      <c r="J30" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30">
+        <v>499600618</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.6">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1926,8 +2123,14 @@
       <c r="I31" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.6">
+      <c r="J31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31">
+        <v>440876102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.6">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1956,8 +2159,14 @@
       <c r="I32" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.6">
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32">
+        <v>463832998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.6">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1986,8 +2195,14 @@
       <c r="I33" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.6">
+      <c r="J33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33">
+        <v>399390808</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.6">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -2016,8 +2231,14 @@
       <c r="I34" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.6">
+      <c r="J34" t="s">
+        <v>35</v>
+      </c>
+      <c r="K34">
+        <v>434938762</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.6">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2046,8 +2267,14 @@
       <c r="I35" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.6">
+      <c r="J35" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35">
+        <v>633099146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.6">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -2076,8 +2303,14 @@
       <c r="I36" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.6">
+      <c r="J36" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36">
+        <v>415343134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.6">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2106,8 +2339,14 @@
       <c r="I37" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.6">
+      <c r="J37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K37">
+        <v>246180126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.6">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -2136,8 +2375,14 @@
       <c r="I38" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.6">
+      <c r="J38" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38">
+        <v>420562172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.6">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2166,8 +2411,14 @@
       <c r="I39" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.6">
+      <c r="J39" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39">
+        <v>328549726</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.6">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2196,8 +2447,14 @@
       <c r="I40" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.6">
+      <c r="J40" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40">
+        <v>390420474</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.6">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -2226,8 +2483,14 @@
       <c r="I41" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.6">
+      <c r="J41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41">
+        <v>266216678</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.6">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -2256,8 +2519,14 @@
       <c r="I42" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.6">
+      <c r="J42" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42">
+        <v>378166292</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.6">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -2286,8 +2555,14 @@
       <c r="I43" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.6">
+      <c r="J43" t="s">
+        <v>44</v>
+      </c>
+      <c r="K43">
+        <v>297158812</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.6">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -2316,8 +2591,14 @@
       <c r="I44" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.6">
+      <c r="J44" t="s">
+        <v>45</v>
+      </c>
+      <c r="K44">
+        <v>264574882</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.6">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2346,8 +2627,14 @@
       <c r="I45" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.6">
+      <c r="J45" t="s">
+        <v>46</v>
+      </c>
+      <c r="K45">
+        <v>164115206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.6">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -2376,8 +2663,14 @@
       <c r="I46" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.6">
+      <c r="J46" t="s">
+        <v>47</v>
+      </c>
+      <c r="K46">
+        <v>288646988</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.6">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -2406,8 +2699,14 @@
       <c r="I47" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.6">
+      <c r="J47" t="s">
+        <v>48</v>
+      </c>
+      <c r="K47">
+        <v>462965648</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.6">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -2436,8 +2735,14 @@
       <c r="I48" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.6">
+      <c r="J48" t="s">
+        <v>49</v>
+      </c>
+      <c r="K48">
+        <v>435687686</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.6">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -2466,8 +2771,14 @@
       <c r="I49" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.6">
+      <c r="J49" t="s">
+        <v>50</v>
+      </c>
+      <c r="K49">
+        <v>475566746</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.6">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2496,8 +2807,14 @@
       <c r="I50" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.6">
+      <c r="J50" t="s">
+        <v>51</v>
+      </c>
+      <c r="K50">
+        <v>459198398</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.6">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -2526,8 +2843,14 @@
       <c r="I51" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.6">
+      <c r="J51" t="s">
+        <v>52</v>
+      </c>
+      <c r="K51">
+        <v>380365534</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.6">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2556,8 +2879,14 @@
       <c r="I52" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.6">
+      <c r="J52" t="s">
+        <v>53</v>
+      </c>
+      <c r="K52">
+        <v>374127914</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15.6">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -2586,8 +2915,14 @@
       <c r="I53" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.6">
+      <c r="J53" t="s">
+        <v>54</v>
+      </c>
+      <c r="K53">
+        <v>417176234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.6">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -2616,8 +2951,14 @@
       <c r="I54" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.6">
+      <c r="J54" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54">
+        <v>306384522</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.6">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -2646,8 +2987,14 @@
       <c r="I55" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.6">
+      <c r="J55" t="s">
+        <v>56</v>
+      </c>
+      <c r="K55">
+        <v>297815870</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.6">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -2676,8 +3023,14 @@
       <c r="I56" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.6">
+      <c r="J56" t="s">
+        <v>57</v>
+      </c>
+      <c r="K56">
+        <v>635896664</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.6">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -2706,8 +3059,14 @@
       <c r="I57" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.6">
+      <c r="J57" t="s">
+        <v>58</v>
+      </c>
+      <c r="K57">
+        <v>371995044</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15.6">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
@@ -2736,8 +3095,14 @@
       <c r="I58" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.6">
+      <c r="J58" t="s">
+        <v>60</v>
+      </c>
+      <c r="K58">
+        <v>398717238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15.6">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
@@ -2766,8 +3131,14 @@
       <c r="I59" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.6">
+      <c r="J59" t="s">
+        <v>61</v>
+      </c>
+      <c r="K59">
+        <v>342284306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.6">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
@@ -2796,8 +3167,14 @@
       <c r="I60" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.6">
+      <c r="J60" t="s">
+        <v>62</v>
+      </c>
+      <c r="K60">
+        <v>368111100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.6">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
@@ -2826,8 +3203,14 @@
       <c r="I61" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15.6">
+      <c r="J61" t="s">
+        <v>63</v>
+      </c>
+      <c r="K61">
+        <v>306153050</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15.6">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
@@ -2856,8 +3239,14 @@
       <c r="I62" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.6">
+      <c r="J62" t="s">
+        <v>64</v>
+      </c>
+      <c r="K62">
+        <v>485136180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="15.6">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -2886,8 +3275,14 @@
       <c r="I63" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.6">
+      <c r="J63" t="s">
+        <v>65</v>
+      </c>
+      <c r="K63">
+        <v>449280384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15.6">
       <c r="A64" s="1" t="s">
         <v>66</v>
       </c>
@@ -2916,8 +3311,14 @@
       <c r="I64" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="15.6">
+      <c r="J64" t="s">
+        <v>66</v>
+      </c>
+      <c r="K64">
+        <v>444691772</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15.6">
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
@@ -2946,8 +3347,14 @@
       <c r="I65" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.6">
+      <c r="J65" t="s">
+        <v>67</v>
+      </c>
+      <c r="K65">
+        <v>269822568</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15.6">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
@@ -2976,8 +3383,14 @@
       <c r="I66" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.6">
+      <c r="J66" t="s">
+        <v>68</v>
+      </c>
+      <c r="K66">
+        <v>442894022</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15.6">
       <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
@@ -3006,8 +3419,14 @@
       <c r="I67" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.6">
+      <c r="J67" t="s">
+        <v>69</v>
+      </c>
+      <c r="K67">
+        <v>402217188</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15.6">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
@@ -3036,8 +3455,14 @@
       <c r="I68" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.6">
+      <c r="J68" t="s">
+        <v>70</v>
+      </c>
+      <c r="K68">
+        <v>437597746</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15.6">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
@@ -3066,8 +3491,14 @@
       <c r="I69" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="15.6">
+      <c r="J69" t="s">
+        <v>71</v>
+      </c>
+      <c r="K69">
+        <v>408885864</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="15.6">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
@@ -3096,8 +3527,14 @@
       <c r="I70" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.6">
+      <c r="J70" t="s">
+        <v>72</v>
+      </c>
+      <c r="K70">
+        <v>338549582</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="15.6">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
@@ -3126,8 +3563,14 @@
       <c r="I71" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.6">
+      <c r="J71" t="s">
+        <v>73</v>
+      </c>
+      <c r="K71">
+        <v>338697124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.6">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
@@ -3156,8 +3599,14 @@
       <c r="I72" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.6">
+      <c r="J72" t="s">
+        <v>74</v>
+      </c>
+      <c r="K72">
+        <v>409640862</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15.6">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
@@ -3186,8 +3635,14 @@
       <c r="I73" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="15.6">
+      <c r="J73" t="s">
+        <v>75</v>
+      </c>
+      <c r="K73">
+        <v>375963270</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="15.6">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
@@ -3216,8 +3671,14 @@
       <c r="I74" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="15.6">
+      <c r="J74" t="s">
+        <v>76</v>
+      </c>
+      <c r="K74">
+        <v>340470354</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="15.6">
       <c r="A75" s="1" t="s">
         <v>77</v>
       </c>
@@ -3246,8 +3707,14 @@
       <c r="I75" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.6">
+      <c r="J75" t="s">
+        <v>77</v>
+      </c>
+      <c r="K75">
+        <v>388403914</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15.6">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
@@ -3276,8 +3743,14 @@
       <c r="I76" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="15.6">
+      <c r="J76" t="s">
+        <v>78</v>
+      </c>
+      <c r="K76">
+        <v>399008374</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="15.6">
       <c r="A77" s="1" t="s">
         <v>79</v>
       </c>
@@ -3306,8 +3779,14 @@
       <c r="I77" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="15.6">
+      <c r="J77" t="s">
+        <v>79</v>
+      </c>
+      <c r="K77">
+        <v>412959348</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.6">
       <c r="A78" s="1" t="s">
         <v>80</v>
       </c>
@@ -3336,8 +3815,14 @@
       <c r="I78" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="15.6">
+      <c r="J78" t="s">
+        <v>80</v>
+      </c>
+      <c r="K78">
+        <v>303174866</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="15.6">
       <c r="A79" s="1" t="s">
         <v>81</v>
       </c>
@@ -3366,8 +3851,14 @@
       <c r="I79" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="15.6">
+      <c r="J79" t="s">
+        <v>81</v>
+      </c>
+      <c r="K79">
+        <v>399549740</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15.6">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
@@ -3396,8 +3887,14 @@
       <c r="I80" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="15.6">
+      <c r="J80" t="s">
+        <v>82</v>
+      </c>
+      <c r="K80">
+        <v>368875202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="15.6">
       <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
@@ -3426,8 +3923,14 @@
       <c r="I81" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="15.6">
+      <c r="J81" t="s">
+        <v>83</v>
+      </c>
+      <c r="K81">
+        <v>373700996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="15.6">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
@@ -3456,8 +3959,14 @@
       <c r="I82" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="15.6">
+      <c r="J82" t="s">
+        <v>84</v>
+      </c>
+      <c r="K82">
+        <v>341739196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="15.6">
       <c r="A83" s="1" t="s">
         <v>85</v>
       </c>
@@ -3486,8 +3995,14 @@
       <c r="I83" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="15.6">
+      <c r="J83" t="s">
+        <v>85</v>
+      </c>
+      <c r="K83">
+        <v>377820080</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="15.6">
       <c r="A84" s="1" t="s">
         <v>86</v>
       </c>
@@ -3516,8 +4031,14 @@
       <c r="I84" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="15.6">
+      <c r="J84" t="s">
+        <v>86</v>
+      </c>
+      <c r="K84">
+        <v>451528640</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="15.6">
       <c r="A85" s="1" t="s">
         <v>87</v>
       </c>
@@ -3546,8 +4067,14 @@
       <c r="I85" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="15.6">
+      <c r="J85" t="s">
+        <v>87</v>
+      </c>
+      <c r="K85">
+        <v>253952482</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="15.6">
       <c r="A86" s="1" t="s">
         <v>88</v>
       </c>
@@ -3576,8 +4103,14 @@
       <c r="I86" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="15.6">
+      <c r="J86" t="s">
+        <v>88</v>
+      </c>
+      <c r="K86">
+        <v>256287760</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="15.6">
       <c r="A87" s="1" t="s">
         <v>89</v>
       </c>
@@ -3606,8 +4139,14 @@
       <c r="I87" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.6">
+      <c r="J87" t="s">
+        <v>89</v>
+      </c>
+      <c r="K87">
+        <v>460018862</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="15.6">
       <c r="A88" s="1" t="s">
         <v>90</v>
       </c>
@@ -3636,8 +4175,14 @@
       <c r="I88" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="15.6">
+      <c r="J88" t="s">
+        <v>90</v>
+      </c>
+      <c r="K88">
+        <v>338611726</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="15.6">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -3666,8 +4211,14 @@
       <c r="I89" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="15.6">
+      <c r="J89" t="s">
+        <v>91</v>
+      </c>
+      <c r="K89">
+        <v>274983484</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="15.6">
       <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
@@ -3696,8 +4247,14 @@
       <c r="I90" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="15.6">
+      <c r="J90" t="s">
+        <v>92</v>
+      </c>
+      <c r="K90">
+        <v>385005800</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="15.6">
       <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
@@ -3726,8 +4283,14 @@
       <c r="I91" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="15.6">
+      <c r="J91" t="s">
+        <v>93</v>
+      </c>
+      <c r="K91">
+        <v>539113764</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="15.6">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -3756,8 +4319,14 @@
       <c r="I92" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="15.6">
+      <c r="J92" t="s">
+        <v>94</v>
+      </c>
+      <c r="K92">
+        <v>359284260</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="15.6">
       <c r="A93" s="1" t="s">
         <v>95</v>
       </c>
@@ -3786,8 +4355,14 @@
       <c r="I93" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="15.6">
+      <c r="J93" t="s">
+        <v>95</v>
+      </c>
+      <c r="K93">
+        <v>437816192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="15.6">
       <c r="A94" s="1" t="s">
         <v>96</v>
       </c>
@@ -3816,8 +4391,14 @@
       <c r="I94" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.6">
+      <c r="J94" t="s">
+        <v>96</v>
+      </c>
+      <c r="K94">
+        <v>321797088</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="15.6">
       <c r="A95" s="1" t="s">
         <v>97</v>
       </c>
@@ -3846,8 +4427,14 @@
       <c r="I95" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="15.6">
+      <c r="J95" t="s">
+        <v>97</v>
+      </c>
+      <c r="K95">
+        <v>423500782</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="15.6">
       <c r="A96" s="1" t="s">
         <v>98</v>
       </c>
@@ -3876,8 +4463,14 @@
       <c r="I96" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="15.6">
+      <c r="J96" t="s">
+        <v>98</v>
+      </c>
+      <c r="K96">
+        <v>278380318</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="15.6">
       <c r="A97" s="1" t="s">
         <v>99</v>
       </c>
@@ -3906,8 +4499,14 @@
       <c r="I97" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="15.6">
+      <c r="J97" t="s">
+        <v>99</v>
+      </c>
+      <c r="K97">
+        <v>328505148</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="15.6">
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
@@ -3936,8 +4535,14 @@
       <c r="I98" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.6">
+      <c r="J98" t="s">
+        <v>100</v>
+      </c>
+      <c r="K98">
+        <v>370803024</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="15.6">
       <c r="A99" s="1" t="s">
         <v>101</v>
       </c>
@@ -3966,8 +4571,14 @@
       <c r="I99" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="15.6">
+      <c r="J99" t="s">
+        <v>101</v>
+      </c>
+      <c r="K99">
+        <v>352030928</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="15.6">
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
@@ -3996,8 +4607,14 @@
       <c r="I100" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="15.6">
+      <c r="J100" t="s">
+        <v>102</v>
+      </c>
+      <c r="K100">
+        <v>354224626</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="15.6">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
@@ -4026,8 +4643,14 @@
       <c r="I101" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="15.6">
+      <c r="J101" t="s">
+        <v>103</v>
+      </c>
+      <c r="K101">
+        <v>307846576</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.6">
       <c r="A102" s="1" t="s">
         <v>104</v>
       </c>
@@ -4056,8 +4679,14 @@
       <c r="I102" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="15.6">
+      <c r="J102" t="s">
+        <v>104</v>
+      </c>
+      <c r="K102">
+        <v>329240054</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="15.6">
       <c r="A103" s="1" t="s">
         <v>105</v>
       </c>
@@ -4086,8 +4715,14 @@
       <c r="I103" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="15.6">
+      <c r="J103" t="s">
+        <v>105</v>
+      </c>
+      <c r="K103">
+        <v>388462874</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="15.6">
       <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
@@ -4116,8 +4751,14 @@
       <c r="I104" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="15.6">
+      <c r="J104" t="s">
+        <v>106</v>
+      </c>
+      <c r="K104">
+        <v>345574560</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="15.6">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
@@ -4146,8 +4787,14 @@
       <c r="I105" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="15.6">
+      <c r="J105" t="s">
+        <v>107</v>
+      </c>
+      <c r="K105">
+        <v>407894524</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="15.6">
       <c r="A106" s="1" t="s">
         <v>108</v>
       </c>
@@ -4176,8 +4823,14 @@
       <c r="I106" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="15.6">
+      <c r="J106" t="s">
+        <v>108</v>
+      </c>
+      <c r="K106">
+        <v>333427578</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="15.6">
       <c r="A107" s="1" t="s">
         <v>109</v>
       </c>
@@ -4206,8 +4859,14 @@
       <c r="I107" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="15.6">
+      <c r="J107" t="s">
+        <v>109</v>
+      </c>
+      <c r="K107">
+        <v>522620482</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="15.6">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
@@ -4236,8 +4895,14 @@
       <c r="I108" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="15.6">
+      <c r="J108" t="s">
+        <v>110</v>
+      </c>
+      <c r="K108">
+        <v>371142378</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="15.6">
       <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
@@ -4266,8 +4931,14 @@
       <c r="I109" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="15.6">
+      <c r="J109" t="s">
+        <v>111</v>
+      </c>
+      <c r="K109">
+        <v>338943134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15.6">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
@@ -4296,8 +4967,14 @@
       <c r="I110" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="15.6">
+      <c r="J110" t="s">
+        <v>112</v>
+      </c>
+      <c r="K110">
+        <v>369538288</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15.6">
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
@@ -4326,8 +5003,14 @@
       <c r="I111" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="15.6">
+      <c r="J111" t="s">
+        <v>113</v>
+      </c>
+      <c r="K111">
+        <v>396286730</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="15.6">
       <c r="A112" s="1" t="s">
         <v>114</v>
       </c>
@@ -4356,8 +5039,14 @@
       <c r="I112" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="15.6">
+      <c r="J112" t="s">
+        <v>114</v>
+      </c>
+      <c r="K112">
+        <v>346238396</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="15.6">
       <c r="A113" s="1" t="s">
         <v>115</v>
       </c>
@@ -4386,8 +5075,14 @@
       <c r="I113" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="15.6">
+      <c r="J113" t="s">
+        <v>115</v>
+      </c>
+      <c r="K113">
+        <v>339721848</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="15.6">
       <c r="A114" s="1" t="s">
         <v>116</v>
       </c>
@@ -4416,8 +5111,14 @@
       <c r="I114" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="15.6">
+      <c r="J114" t="s">
+        <v>116</v>
+      </c>
+      <c r="K114">
+        <v>357891876</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="15.6">
       <c r="A115" s="1" t="s">
         <v>117</v>
       </c>
@@ -4446,8 +5147,14 @@
       <c r="I115" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="15.6">
+      <c r="J115" t="s">
+        <v>117</v>
+      </c>
+      <c r="K115">
+        <v>388065794</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="15.6">
       <c r="A116" s="1" t="s">
         <v>118</v>
       </c>
@@ -4476,8 +5183,14 @@
       <c r="I116" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="15.6">
+      <c r="J116" t="s">
+        <v>118</v>
+      </c>
+      <c r="K116">
+        <v>387769558</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="15.6">
       <c r="A117" s="1" t="s">
         <v>119</v>
       </c>
@@ -4506,8 +5219,14 @@
       <c r="I117" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="15.6">
+      <c r="J117" t="s">
+        <v>119</v>
+      </c>
+      <c r="K117">
+        <v>364054734</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="15.6">
       <c r="A118" s="1" t="s">
         <v>120</v>
       </c>
@@ -4536,8 +5255,14 @@
       <c r="I118" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="15.6">
+      <c r="J118" t="s">
+        <v>120</v>
+      </c>
+      <c r="K118">
+        <v>342398030</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="15.6">
       <c r="A119" s="1" t="s">
         <v>121</v>
       </c>
@@ -4566,8 +5291,14 @@
       <c r="I119" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="15.6">
+      <c r="J119" t="s">
+        <v>121</v>
+      </c>
+      <c r="K119">
+        <v>385071042</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="15.6">
       <c r="A120" s="1" t="s">
         <v>122</v>
       </c>
@@ -4596,8 +5327,14 @@
       <c r="I120" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="15.6">
+      <c r="J120" t="s">
+        <v>122</v>
+      </c>
+      <c r="K120">
+        <v>402714396</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="15.6">
       <c r="A121" s="1" t="s">
         <v>123</v>
       </c>
@@ -4626,8 +5363,14 @@
       <c r="I121" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="15.6">
+      <c r="J121" t="s">
+        <v>123</v>
+      </c>
+      <c r="K121">
+        <v>342278366</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="15.6">
       <c r="A122" s="1" t="s">
         <v>124</v>
       </c>
@@ -4656,8 +5399,14 @@
       <c r="I122" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="15.6">
+      <c r="J122" t="s">
+        <v>124</v>
+      </c>
+      <c r="K122">
+        <v>391822972</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="15.6">
       <c r="A123" s="1" t="s">
         <v>125</v>
       </c>
@@ -4686,8 +5435,14 @@
       <c r="I123" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="15.6">
+      <c r="J123" t="s">
+        <v>125</v>
+      </c>
+      <c r="K123">
+        <v>346225714</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="15.6">
       <c r="A124" s="1" t="s">
         <v>126</v>
       </c>
@@ -4716,8 +5471,14 @@
       <c r="I124" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="15.6">
+      <c r="J124" t="s">
+        <v>126</v>
+      </c>
+      <c r="K124">
+        <v>370334582</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="15.6">
       <c r="A125" s="1" t="s">
         <v>127</v>
       </c>
@@ -4746,8 +5507,14 @@
       <c r="I125" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="15.6">
+      <c r="J125" t="s">
+        <v>127</v>
+      </c>
+      <c r="K125">
+        <v>328237008</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="15.6">
       <c r="A126" s="1" t="s">
         <v>128</v>
       </c>
@@ -4776,8 +5543,14 @@
       <c r="I126" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="15.6">
+      <c r="J126" t="s">
+        <v>128</v>
+      </c>
+      <c r="K126">
+        <v>314283624</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" ht="15.6">
       <c r="A127" s="1" t="s">
         <v>129</v>
       </c>
@@ -4806,8 +5579,14 @@
       <c r="I127" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="15.6">
+      <c r="J127" t="s">
+        <v>129</v>
+      </c>
+      <c r="K127">
+        <v>311581824</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="15.6">
       <c r="A128" s="1" t="s">
         <v>130</v>
       </c>
@@ -4836,8 +5615,14 @@
       <c r="I128" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" ht="15.6">
+      <c r="J128" t="s">
+        <v>130</v>
+      </c>
+      <c r="K128">
+        <v>397681922</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="15.6">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -4866,8 +5651,14 @@
       <c r="I129" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="15.6">
+      <c r="J129" t="s">
+        <v>131</v>
+      </c>
+      <c r="K129">
+        <v>357393502</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="15.6">
       <c r="A130" s="1" t="s">
         <v>132</v>
       </c>
@@ -4896,8 +5687,14 @@
       <c r="I130" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" ht="15.6">
+      <c r="J130" t="s">
+        <v>132</v>
+      </c>
+      <c r="K130">
+        <v>370391086</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" ht="15.6">
       <c r="A131" s="1" t="s">
         <v>133</v>
       </c>
@@ -4926,8 +5723,14 @@
       <c r="I131" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" ht="15.6">
+      <c r="J131" t="s">
+        <v>133</v>
+      </c>
+      <c r="K131">
+        <v>281316518</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="15.6">
       <c r="A132" s="1" t="s">
         <v>134</v>
       </c>
@@ -4956,8 +5759,14 @@
       <c r="I132" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.6">
+      <c r="J132" t="s">
+        <v>134</v>
+      </c>
+      <c r="K132">
+        <v>322501268</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" ht="15.6">
       <c r="A133" s="1" t="s">
         <v>136</v>
       </c>
@@ -4986,8 +5795,14 @@
       <c r="I133" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" ht="15.6">
+      <c r="J133" t="s">
+        <v>136</v>
+      </c>
+      <c r="K133">
+        <v>339465160</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" ht="15.6">
       <c r="A134" s="1" t="s">
         <v>137</v>
       </c>
@@ -5016,8 +5831,14 @@
       <c r="I134" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" ht="15.6">
+      <c r="J134" t="s">
+        <v>137</v>
+      </c>
+      <c r="K134">
+        <v>342121874</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="15.6">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -5046,8 +5867,14 @@
       <c r="I135" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" ht="15.6">
+      <c r="J135" t="s">
+        <v>138</v>
+      </c>
+      <c r="K135">
+        <v>318044830</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" ht="15.6">
       <c r="A136" s="1" t="s">
         <v>139</v>
       </c>
@@ -5076,8 +5903,14 @@
       <c r="I136" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" ht="15.6">
+      <c r="J136" t="s">
+        <v>139</v>
+      </c>
+      <c r="K136">
+        <v>263756272</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" ht="15.6">
       <c r="A137" s="1" t="s">
         <v>140</v>
       </c>
@@ -5106,8 +5939,14 @@
       <c r="I137" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" ht="15.6">
+      <c r="J137" t="s">
+        <v>140</v>
+      </c>
+      <c r="K137">
+        <v>351574504</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" ht="15.6">
       <c r="A138" s="1" t="s">
         <v>141</v>
       </c>
@@ -5136,8 +5975,14 @@
       <c r="I138" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" ht="15.6">
+      <c r="J138" t="s">
+        <v>141</v>
+      </c>
+      <c r="K138">
+        <v>327623186</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" ht="15.6">
       <c r="A139" s="1" t="s">
         <v>142</v>
       </c>
@@ -5166,8 +6011,14 @@
       <c r="I139" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" ht="15.6">
+      <c r="J139" t="s">
+        <v>142</v>
+      </c>
+      <c r="K139">
+        <v>440972758</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" ht="15.6">
       <c r="A140" s="1" t="s">
         <v>143</v>
       </c>
@@ -5196,8 +6047,14 @@
       <c r="I140" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" ht="15.6">
+      <c r="J140" t="s">
+        <v>143</v>
+      </c>
+      <c r="K140">
+        <v>336511738</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" ht="15.6">
       <c r="A141" s="1" t="s">
         <v>144</v>
       </c>
@@ -5226,8 +6083,14 @@
       <c r="I141" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" ht="15.6">
+      <c r="J141" t="s">
+        <v>144</v>
+      </c>
+      <c r="K141">
+        <v>386120244</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" ht="15.6">
       <c r="A142" s="1" t="s">
         <v>145</v>
       </c>
@@ -5256,8 +6119,14 @@
       <c r="I142" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" ht="15.6">
+      <c r="J142" t="s">
+        <v>145</v>
+      </c>
+      <c r="K142">
+        <v>404391722</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" ht="15.6">
       <c r="A143" s="1" t="s">
         <v>146</v>
       </c>
@@ -5286,8 +6155,14 @@
       <c r="I143" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" ht="15.6">
+      <c r="J143" t="s">
+        <v>146</v>
+      </c>
+      <c r="K143">
+        <v>338171936</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="15.6">
       <c r="A144" s="1" t="s">
         <v>147</v>
       </c>
@@ -5316,8 +6191,14 @@
       <c r="I144" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" ht="15.6">
+      <c r="J144" t="s">
+        <v>147</v>
+      </c>
+      <c r="K144">
+        <v>324346516</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="15.6">
       <c r="A145" s="1" t="s">
         <v>148</v>
       </c>
@@ -5346,8 +6227,14 @@
       <c r="I145" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" ht="15.6">
+      <c r="J145" t="s">
+        <v>148</v>
+      </c>
+      <c r="K145">
+        <v>282805050</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="15.6">
       <c r="A146" s="1" t="s">
         <v>149</v>
       </c>
@@ -5376,8 +6263,14 @@
       <c r="I146" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" ht="15.6">
+      <c r="J146" t="s">
+        <v>149</v>
+      </c>
+      <c r="K146">
+        <v>324132078</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" ht="15.6">
       <c r="A147" s="1" t="s">
         <v>150</v>
       </c>
@@ -5406,8 +6299,14 @@
       <c r="I147" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" ht="15.6">
+      <c r="J147" t="s">
+        <v>150</v>
+      </c>
+      <c r="K147">
+        <v>342014496</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" ht="15.6">
       <c r="A148" s="1" t="s">
         <v>151</v>
       </c>
@@ -5436,8 +6335,14 @@
       <c r="I148" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" ht="15.6">
+      <c r="J148" t="s">
+        <v>151</v>
+      </c>
+      <c r="K148">
+        <v>359981962</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="15.6">
       <c r="A149" s="1" t="s">
         <v>152</v>
       </c>
@@ -5466,8 +6371,14 @@
       <c r="I149" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" ht="15.6">
+      <c r="J149" t="s">
+        <v>152</v>
+      </c>
+      <c r="K149">
+        <v>323196296</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" ht="15.6">
       <c r="A150" s="1" t="s">
         <v>153</v>
       </c>
@@ -5496,8 +6407,14 @@
       <c r="I150" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" ht="15.6">
+      <c r="J150" t="s">
+        <v>153</v>
+      </c>
+      <c r="K150">
+        <v>320960112</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="15.6">
       <c r="A151" s="1" t="s">
         <v>154</v>
       </c>
@@ -5526,8 +6443,14 @@
       <c r="I151" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" ht="15.6">
+      <c r="J151" t="s">
+        <v>154</v>
+      </c>
+      <c r="K151">
+        <v>295539040</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" ht="15.6">
       <c r="A152" s="1" t="s">
         <v>155</v>
       </c>
@@ -5556,8 +6479,14 @@
       <c r="I152" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" ht="15.6">
+      <c r="J152" t="s">
+        <v>155</v>
+      </c>
+      <c r="K152">
+        <v>321829274</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="15.6">
       <c r="A153" s="1" t="s">
         <v>156</v>
       </c>
@@ -5586,8 +6515,14 @@
       <c r="I153" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" ht="15.6">
+      <c r="J153" t="s">
+        <v>156</v>
+      </c>
+      <c r="K153">
+        <v>351923732</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="15.6">
       <c r="A154" s="1" t="s">
         <v>157</v>
       </c>
@@ -5616,8 +6551,14 @@
       <c r="I154" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" ht="15.6">
+      <c r="J154" t="s">
+        <v>157</v>
+      </c>
+      <c r="K154">
+        <v>387847764</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="15.6">
       <c r="A155" s="1" t="s">
         <v>158</v>
       </c>
@@ -5646,8 +6587,14 @@
       <c r="I155" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" ht="15.6">
+      <c r="J155" t="s">
+        <v>158</v>
+      </c>
+      <c r="K155">
+        <v>304256672</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="15.6">
       <c r="A156" s="1" t="s">
         <v>159</v>
       </c>
@@ -5676,8 +6623,14 @@
       <c r="I156" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" ht="15.6">
+      <c r="J156" t="s">
+        <v>159</v>
+      </c>
+      <c r="K156">
+        <v>347699812</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="15.6">
       <c r="A157" s="1" t="s">
         <v>160</v>
       </c>
@@ -5706,8 +6659,14 @@
       <c r="I157" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" ht="15.6">
+      <c r="J157" t="s">
+        <v>160</v>
+      </c>
+      <c r="K157">
+        <v>388341000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="15.6">
       <c r="A158" s="1" t="s">
         <v>161</v>
       </c>
@@ -5736,8 +6695,14 @@
       <c r="I158" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" ht="15.6">
+      <c r="J158" t="s">
+        <v>161</v>
+      </c>
+      <c r="K158">
+        <v>361095072</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="15.6">
       <c r="A159" s="1" t="s">
         <v>162</v>
       </c>
@@ -5766,8 +6731,14 @@
       <c r="I159" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" ht="15.6">
+      <c r="J159" t="s">
+        <v>162</v>
+      </c>
+      <c r="K159">
+        <v>482084694</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="15.6">
       <c r="A160" s="1" t="s">
         <v>163</v>
       </c>
@@ -5796,8 +6767,14 @@
       <c r="I160" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" ht="15.6">
+      <c r="J160" t="s">
+        <v>163</v>
+      </c>
+      <c r="K160">
+        <v>410083042</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="15.6">
       <c r="A161" s="1" t="s">
         <v>164</v>
       </c>
@@ -5826,8 +6803,14 @@
       <c r="I161" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" ht="15.6">
+      <c r="J161" t="s">
+        <v>164</v>
+      </c>
+      <c r="K161">
+        <v>327742496</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" ht="15.6">
       <c r="A162" s="1" t="s">
         <v>165</v>
       </c>
@@ -5856,8 +6839,14 @@
       <c r="I162" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" ht="15.6">
+      <c r="J162" t="s">
+        <v>165</v>
+      </c>
+      <c r="K162">
+        <v>403570132</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" ht="15.6">
       <c r="A163" s="1" t="s">
         <v>166</v>
       </c>
@@ -5886,8 +6875,14 @@
       <c r="I163" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" ht="15.6">
+      <c r="J163" t="s">
+        <v>166</v>
+      </c>
+      <c r="K163">
+        <v>419019388</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="15.6">
       <c r="A164" s="1" t="s">
         <v>167</v>
       </c>
@@ -5916,8 +6911,14 @@
       <c r="I164" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" ht="15.6">
+      <c r="J164" t="s">
+        <v>167</v>
+      </c>
+      <c r="K164">
+        <v>324730830</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" ht="15.6">
       <c r="A165" s="1" t="s">
         <v>168</v>
       </c>
@@ -5946,8 +6947,14 @@
       <c r="I165" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" ht="15.6">
+      <c r="J165" t="s">
+        <v>168</v>
+      </c>
+      <c r="K165">
+        <v>402932612</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" ht="15.6">
       <c r="A166" s="1" t="s">
         <v>169</v>
       </c>
@@ -5976,8 +6983,14 @@
       <c r="I166" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" ht="15.6">
+      <c r="J166" t="s">
+        <v>169</v>
+      </c>
+      <c r="K166">
+        <v>304435280</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" ht="15.6">
       <c r="A167" s="1" t="s">
         <v>170</v>
       </c>
@@ -6006,8 +7019,14 @@
       <c r="I167" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" ht="15.6">
+      <c r="J167" t="s">
+        <v>170</v>
+      </c>
+      <c r="K167">
+        <v>291324614</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="15.6">
       <c r="A168" s="1" t="s">
         <v>171</v>
       </c>
@@ -6036,8 +7055,14 @@
       <c r="I168" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" ht="15.6">
+      <c r="J168" t="s">
+        <v>171</v>
+      </c>
+      <c r="K168">
+        <v>324989054</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" ht="15.6">
       <c r="A169" s="1" t="s">
         <v>172</v>
       </c>
@@ -6066,8 +7091,14 @@
       <c r="I169" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" ht="15.6">
+      <c r="J169" t="s">
+        <v>172</v>
+      </c>
+      <c r="K169">
+        <v>151825104</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" ht="15.6">
       <c r="A170" s="1" t="s">
         <v>173</v>
       </c>
@@ -6096,8 +7127,14 @@
       <c r="I170" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" ht="15.6">
+      <c r="J170" t="s">
+        <v>173</v>
+      </c>
+      <c r="K170">
+        <v>149845934</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" ht="15.6">
       <c r="A171" s="1" t="s">
         <v>174</v>
       </c>
@@ -6126,8 +7163,14 @@
       <c r="I171" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" ht="15.6">
+      <c r="J171" t="s">
+        <v>174</v>
+      </c>
+      <c r="K171">
+        <v>458295920</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" ht="15.6">
       <c r="A172" s="1" t="s">
         <v>175</v>
       </c>
@@ -6156,8 +7199,14 @@
       <c r="I172" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" ht="15.6">
+      <c r="J172" t="s">
+        <v>175</v>
+      </c>
+      <c r="K172">
+        <v>387230740</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" ht="15.6">
       <c r="A173" s="1" t="s">
         <v>176</v>
       </c>
@@ -6186,8 +7235,14 @@
       <c r="I173" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" ht="15.6">
+      <c r="J173" t="s">
+        <v>176</v>
+      </c>
+      <c r="K173">
+        <v>408427272</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" ht="15.6">
       <c r="A174" s="1" t="s">
         <v>177</v>
       </c>
@@ -6213,8 +7268,14 @@
       <c r="I174" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" ht="15.6">
+      <c r="J174" t="s">
+        <v>177</v>
+      </c>
+      <c r="K174">
+        <v>476921334</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" ht="15.6">
       <c r="A175" s="1" t="s">
         <v>178</v>
       </c>
@@ -6240,8 +7301,14 @@
       <c r="I175" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" ht="15.6">
+      <c r="J175" t="s">
+        <v>178</v>
+      </c>
+      <c r="K175">
+        <v>489617426</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" ht="15.6">
       <c r="A176" s="1" t="s">
         <v>179</v>
       </c>
@@ -6267,8 +7334,14 @@
       <c r="I176" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" ht="15.6">
+      <c r="J176" t="s">
+        <v>179</v>
+      </c>
+      <c r="K176">
+        <v>416553274</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" ht="15.6">
       <c r="A177" s="1" t="s">
         <v>180</v>
       </c>
@@ -6297,8 +7370,14 @@
       <c r="I177" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" ht="15.6">
+      <c r="J177" t="s">
+        <v>180</v>
+      </c>
+      <c r="K177">
+        <v>252063110</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" ht="15.6">
       <c r="A178" s="1" t="s">
         <v>181</v>
       </c>
@@ -6327,8 +7406,14 @@
       <c r="I178" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" ht="15.6">
+      <c r="J178" t="s">
+        <v>181</v>
+      </c>
+      <c r="K178">
+        <v>277574946</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" ht="15.6">
       <c r="A179" s="1" t="s">
         <v>182</v>
       </c>
@@ -6357,8 +7442,14 @@
       <c r="I179" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" ht="15.6">
+      <c r="J179" t="s">
+        <v>182</v>
+      </c>
+      <c r="K179">
+        <v>262268056</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" ht="15.6">
       <c r="A180" s="1" t="s">
         <v>183</v>
       </c>
@@ -6387,8 +7478,14 @@
       <c r="I180" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" ht="15.6">
+      <c r="J180" t="s">
+        <v>183</v>
+      </c>
+      <c r="K180">
+        <v>260588896</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" ht="15.6">
       <c r="A181" s="1" t="s">
         <v>184</v>
       </c>
@@ -6414,8 +7511,14 @@
       <c r="I181" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" ht="15.6">
+      <c r="J181" t="s">
+        <v>184</v>
+      </c>
+      <c r="K181">
+        <v>404962514</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" ht="15.6">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>

</xml_diff>

<commit_message>
rediscover 5-20 micron samples
</commit_message>
<xml_diff>
--- a/Figure Generating/data/DNA_Location_Metadata.xlsx
+++ b/Figure Generating/data/DNA_Location_Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Juntao\Desktop\transposase-deep-ocean\Figure Generating\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F01CA8F-B738-4EC5-AE50-31143D26F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67F9A7F-0CB1-40A5-BC2F-BE670EC30159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21360" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="386">
   <si>
     <t>TARA_A100000164</t>
   </si>
@@ -1192,6 +1192,9 @@
   </si>
   <si>
     <t>ERR598999|ERR599033|ERR599083|ERR599096</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
 </sst>
 </file>
@@ -1259,11 +1262,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1549,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K304"/>
+  <dimension ref="A1:L304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1560,10 +1562,11 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6">
+    <row r="1" spans="1:12" ht="15.6">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -1573,32 +1576,35 @@
       <c r="C1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6">
+    <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,17 +1630,20 @@
       <c r="H2">
         <v>208.245</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>21.486650000000001</v>
+      </c>
+      <c r="J2" t="s">
         <v>194</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>415570856</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6">
+    <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1660,17 +1669,20 @@
       <c r="H3">
         <v>218.75115</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>18.616209999999999</v>
+      </c>
+      <c r="J3" t="s">
         <v>194</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>367820654</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6">
+    <row r="4" spans="1:12" ht="15.6">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1696,17 +1708,20 @@
       <c r="H4">
         <v>207.61355</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <v>20.442499999999999</v>
+      </c>
+      <c r="J4" t="s">
         <v>194</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>488612256</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6">
+    <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1732,17 +1747,20 @@
       <c r="H5">
         <v>188.341917</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5">
+        <v>25.811707999999999</v>
+      </c>
+      <c r="J5" t="s">
         <v>186</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>398181184</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6">
+    <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1768,17 +1786,20 @@
       <c r="H6">
         <v>181.501</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6">
+        <v>26.129249999999999</v>
+      </c>
+      <c r="J6" t="s">
         <v>186</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>394451818</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6">
+    <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1804,17 +1825,20 @@
       <c r="H7">
         <v>183.589125</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7">
+        <v>27.309699999999999</v>
+      </c>
+      <c r="J7" t="s">
         <v>186</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>255740402</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6">
+    <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1840,17 +1864,20 @@
       <c r="H8">
         <v>189.91675000000001</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8">
+        <v>25.028099999999998</v>
+      </c>
+      <c r="J8" t="s">
         <v>186</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>403538306</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6">
+    <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1873,17 +1900,20 @@
         <f t="shared" si="0"/>
         <v>0.95424250943932487</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9">
+        <v>23.8141</v>
+      </c>
+      <c r="J9" t="s">
         <v>194</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>221166612</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6">
+    <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1906,17 +1936,20 @@
         <f t="shared" si="0"/>
         <v>1.6232492903979006</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10">
+        <v>17.521075</v>
+      </c>
+      <c r="J10" t="s">
         <v>194</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>178519830</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.6">
+    <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1942,17 +1975,20 @@
       <c r="H11">
         <v>207.5812</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11">
+        <v>21.763570000000001</v>
+      </c>
+      <c r="J11" t="s">
         <v>201</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>291527114</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.6">
+    <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1978,17 +2014,20 @@
       <c r="H12">
         <v>207.48285000000001</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12">
+        <v>21.72823</v>
+      </c>
+      <c r="J12" t="s">
         <v>201</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>436200002</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6">
+    <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2014,17 +2053,20 @@
       <c r="H13">
         <v>199.726</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13">
+        <v>8.3303499999999993</v>
+      </c>
+      <c r="J13" t="s">
         <v>201</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>447472502</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.6">
+    <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2050,17 +2092,20 @@
       <c r="H14">
         <v>239.93725000000001</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14">
+        <v>15.013362000000001</v>
+      </c>
+      <c r="J14" t="s">
         <v>195</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>323328644</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.6">
+    <row r="15" spans="1:12" ht="15.6">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2086,17 +2131,20 @@
       <c r="H15">
         <v>239.79106300000001</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15">
+        <v>15.013999999999999</v>
+      </c>
+      <c r="J15" t="s">
         <v>195</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>151854660</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6">
+    <row r="16" spans="1:12" ht="15.6">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2119,17 +2167,17 @@
         <f t="shared" si="0"/>
         <v>0.69897000433601886</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>201</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>291429494</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.6">
+    <row r="17" spans="1:12" ht="15.6">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2155,17 +2203,20 @@
       <c r="H17">
         <v>181.10193799999999</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17">
+        <v>25.113924999999998</v>
+      </c>
+      <c r="J17" t="s">
         <v>201</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>337711862</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6">
+    <row r="18" spans="1:12" ht="15.6">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2191,17 +2242,20 @@
       <c r="H18">
         <v>194.06091699999999</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18">
+        <v>26.553474999999999</v>
+      </c>
+      <c r="J18" t="s">
         <v>201</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>336385740</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6">
+    <row r="19" spans="1:12" ht="15.6">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2227,17 +2281,20 @@
       <c r="H19">
         <v>193.16499999999999</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19">
+        <v>27.296125</v>
+      </c>
+      <c r="J19" t="s">
         <v>201</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>324775688</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6">
+    <row r="20" spans="1:12" ht="15.6">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2263,17 +2320,20 @@
       <c r="H20">
         <v>183.84625</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20">
+        <v>27.635024999999999</v>
+      </c>
+      <c r="J20" t="s">
         <v>186</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>241970908</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.6">
+    <row r="21" spans="1:12" ht="15.6">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2299,17 +2359,20 @@
       <c r="H21">
         <v>175.50899999999999</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21">
+        <v>27.558762999999999</v>
+      </c>
+      <c r="J21" t="s">
         <v>186</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>450135214</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.6">
+    <row r="22" spans="1:12" ht="15.6">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2335,17 +2398,20 @@
       <c r="H22">
         <v>206.56883300000001</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22">
+        <v>25.329231</v>
+      </c>
+      <c r="J22" t="s">
         <v>201</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>402672664</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.6">
+    <row r="23" spans="1:12" ht="15.6">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2371,17 +2437,20 @@
       <c r="H23">
         <v>189.02330000000001</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23">
+        <v>25.607735000000002</v>
+      </c>
+      <c r="J23" t="s">
         <v>201</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>420102752</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.6">
+    <row r="24" spans="1:12" ht="15.6">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2407,17 +2476,20 @@
       <c r="H24">
         <v>187.47614999999999</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24">
+        <v>26.692435</v>
+      </c>
+      <c r="J24" t="s">
         <v>201</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>338044892</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.6">
+    <row r="25" spans="1:12" ht="15.6">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2443,17 +2515,20 @@
       <c r="H25">
         <v>188.79575</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25">
+        <v>30.127849999999999</v>
+      </c>
+      <c r="J25" t="s">
         <v>201</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>402211598</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.6">
+    <row r="26" spans="1:12" ht="15.6">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -2479,17 +2554,20 @@
       <c r="H26">
         <v>137.99808300000001</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26">
+        <v>27.956099999999999</v>
+      </c>
+      <c r="J26" t="s">
         <v>201</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>430413408</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.6">
+    <row r="27" spans="1:12" ht="15.6">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -2515,17 +2593,20 @@
       <c r="H27">
         <v>186.0215</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27">
+        <v>30.593450000000001</v>
+      </c>
+      <c r="J27" t="s">
         <v>201</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>391430950</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.6">
+    <row r="28" spans="1:12" ht="15.6">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2551,17 +2632,20 @@
       <c r="H28">
         <v>191.628083</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28">
+        <v>27.956482999999999</v>
+      </c>
+      <c r="J28" t="s">
         <v>201</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>404906778</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.6">
+    <row r="29" spans="1:12" ht="15.6">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -2587,17 +2671,20 @@
       <c r="H29">
         <v>194.81774999999999</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29">
+        <v>25.212641999999999</v>
+      </c>
+      <c r="J29" t="s">
         <v>201</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>389259730</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.6">
+    <row r="30" spans="1:12" ht="15.6">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -2623,17 +2710,20 @@
       <c r="H30">
         <v>187.35</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30">
+        <v>29.818107999999999</v>
+      </c>
+      <c r="J30" t="s">
         <v>201</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>499600618</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.6">
+    <row r="31" spans="1:12" ht="15.6">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2659,17 +2749,20 @@
       <c r="H31">
         <v>187.306625</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31">
+        <v>29.151544000000001</v>
+      </c>
+      <c r="J31" t="s">
         <v>201</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>440876102</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.6">
+    <row r="32" spans="1:12" ht="15.6">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2695,17 +2788,20 @@
       <c r="H32">
         <v>164.44006300000001</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32">
+        <v>27.374181</v>
+      </c>
+      <c r="J32" t="s">
         <v>201</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>463832998</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.6">
+    <row r="33" spans="1:12" ht="15.6">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2731,17 +2827,20 @@
       <c r="H33">
         <v>2.8162500000000001</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33">
+        <v>11.984006000000001</v>
+      </c>
+      <c r="J33" t="s">
         <v>201</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>399390808</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.6">
+    <row r="34" spans="1:12" ht="15.6">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -2767,17 +2866,20 @@
       <c r="H34">
         <v>88.889750000000006</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34">
+        <v>6.1957750000000003</v>
+      </c>
+      <c r="J34" t="s">
         <v>201</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>434938762</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.6">
+    <row r="35" spans="1:12" ht="15.6">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2803,17 +2905,20 @@
       <c r="H35">
         <v>210.23949999999999</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35">
+        <v>22.241399999999999</v>
+      </c>
+      <c r="J35" t="s">
         <v>201</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>633099146</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.6">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -2839,17 +2944,20 @@
       <c r="H36">
         <v>207.95660000000001</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36">
+        <v>22.215305000000001</v>
+      </c>
+      <c r="J36" t="s">
         <v>201</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>415343134</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.6">
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2875,17 +2983,20 @@
       <c r="H37">
         <v>190.888667</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37">
+        <v>7.5520170000000002</v>
+      </c>
+      <c r="J37" t="s">
         <v>201</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>246180126</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.6">
+    <row r="38" spans="1:12" ht="15.6">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -2911,17 +3022,20 @@
       <c r="H38">
         <v>199.13499999999999</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38">
+        <v>25.064425</v>
+      </c>
+      <c r="J38" t="s">
         <v>195</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>420562172</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.6">
+    <row r="39" spans="1:12" ht="15.6">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2947,17 +3061,20 @@
       <c r="H39">
         <v>190.5966</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39">
+        <v>23.630095000000001</v>
+      </c>
+      <c r="J39" t="s">
         <v>195</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>328549726</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.6">
+    <row r="40" spans="1:12" ht="15.6">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2983,17 +3100,20 @@
       <c r="H40">
         <v>161.92525000000001</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40">
+        <v>4.188237</v>
+      </c>
+      <c r="J40" t="s">
         <v>195</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>390420474</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.6">
+    <row r="41" spans="1:12" ht="15.6">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -3019,17 +3139,20 @@
       <c r="H41">
         <v>215.20070000000001</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41">
+        <v>19.770009999999999</v>
+      </c>
+      <c r="J41" t="s">
         <v>195</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>266216678</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.6">
+    <row r="42" spans="1:12" ht="15.6">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -3055,17 +3178,20 @@
       <c r="H42">
         <v>194.4342</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42">
+        <v>7.3214499999999996</v>
+      </c>
+      <c r="J42" t="s">
         <v>195</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>378166292</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.6">
+    <row r="43" spans="1:12" ht="15.6">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -3091,17 +3217,20 @@
       <c r="H43">
         <v>234.47630000000001</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43">
+        <v>16.863199999999999</v>
+      </c>
+      <c r="J43" t="s">
         <v>195</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>297158812</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.6">
+    <row r="44" spans="1:12" ht="15.6">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -3127,17 +3256,20 @@
       <c r="H44">
         <v>231.97739999999999</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44">
+        <v>16.74878</v>
+      </c>
+      <c r="J44" t="s">
         <v>195</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>264574882</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.6">
+    <row r="45" spans="1:12" ht="15.6">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -3163,17 +3295,20 @@
       <c r="H45">
         <v>252.63145</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45">
+        <v>13.04322</v>
+      </c>
+      <c r="J45" t="s">
         <v>195</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>164115206</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.6">
+    <row r="46" spans="1:12" ht="15.6">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -3199,17 +3334,20 @@
       <c r="H46">
         <v>143.27362500000001</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46">
+        <v>4.6417190000000002</v>
+      </c>
+      <c r="J46" t="s">
         <v>195</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>288646988</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.6">
+    <row r="47" spans="1:12" ht="15.6">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -3235,17 +3373,20 @@
       <c r="H47">
         <v>206.23185000000001</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47">
+        <v>23.374825000000001</v>
+      </c>
+      <c r="J47" t="s">
         <v>195</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>462965648</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.6">
+    <row r="48" spans="1:12" ht="15.6">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -3271,17 +3412,20 @@
       <c r="H48">
         <v>200.32464999999999</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48">
+        <v>21.165959999999998</v>
+      </c>
+      <c r="J48" t="s">
         <v>195</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>435687686</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.6">
+    <row r="49" spans="1:12" ht="15.6">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -3307,17 +3451,20 @@
       <c r="H49">
         <v>221.13845000000001</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49">
+        <v>20.077750000000002</v>
+      </c>
+      <c r="J49" t="s">
         <v>195</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>475566746</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.6">
+    <row r="50" spans="1:12" ht="15.6">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -3343,17 +3490,20 @@
       <c r="H50">
         <v>216.65469999999999</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50">
+        <v>19.323350000000001</v>
+      </c>
+      <c r="J50" t="s">
         <v>195</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>459198398</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.6">
+    <row r="51" spans="1:12" ht="15.6">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -3379,17 +3529,20 @@
       <c r="H51">
         <v>209.1003</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51">
+        <v>22.781829999999999</v>
+      </c>
+      <c r="J51" t="s">
         <v>196</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>380365534</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.6">
+    <row r="52" spans="1:12" ht="15.6">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -3415,17 +3568,20 @@
       <c r="H52">
         <v>208.54894999999999</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52">
+        <v>19.783275</v>
+      </c>
+      <c r="J52" t="s">
         <v>196</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>374127914</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.6">
+    <row r="53" spans="1:12" ht="15.6">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -3451,17 +3607,20 @@
       <c r="H53">
         <v>4.7046999999999999</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53">
+        <v>10.69894</v>
+      </c>
+      <c r="J53" t="s">
         <v>196</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>417176234</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6">
+    <row r="54" spans="1:12" ht="15.6">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -3487,17 +3646,20 @@
       <c r="H54">
         <v>180.67375000000001</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54">
+        <v>26.218437999999999</v>
+      </c>
+      <c r="J54" t="s">
         <v>196</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>306384522</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.6">
+    <row r="55" spans="1:12" ht="15.6">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -3523,17 +3685,20 @@
       <c r="H55">
         <v>177.67306300000001</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55">
+        <v>26.139288000000001</v>
+      </c>
+      <c r="J55" t="s">
         <v>196</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>297815870</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.6">
+    <row r="56" spans="1:12" ht="15.6">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -3559,17 +3724,20 @@
       <c r="H56">
         <v>190.378187</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56">
+        <v>26.572419</v>
+      </c>
+      <c r="J56" t="s">
         <v>196</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>635896664</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.6">
+    <row r="57" spans="1:12" ht="15.6">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -3595,17 +3763,20 @@
       <c r="H57">
         <v>172.42474999999999</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57">
+        <v>24.813970000000001</v>
+      </c>
+      <c r="J57" t="s">
         <v>196</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>371995044</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15.6">
+    <row r="58" spans="1:12" ht="15.6">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
@@ -3631,17 +3802,20 @@
       <c r="H58">
         <v>40.610700000000001</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58">
+        <v>7.1339949999999996</v>
+      </c>
+      <c r="J58" t="s">
         <v>196</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>398717238</v>
       </c>
-      <c r="K58" t="s">
+      <c r="L58" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.6">
+    <row r="59" spans="1:12" ht="15.6">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
@@ -3667,17 +3841,20 @@
       <c r="H59">
         <v>189.67009999999999</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59">
+        <v>26.586684999999999</v>
+      </c>
+      <c r="J59" t="s">
         <v>196</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>342284306</v>
       </c>
-      <c r="K59" t="s">
+      <c r="L59" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.6">
+    <row r="60" spans="1:12" ht="15.6">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
@@ -3703,17 +3880,20 @@
       <c r="H60">
         <v>158.18405000000001</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60">
+        <v>21.97372</v>
+      </c>
+      <c r="J60" t="s">
         <v>196</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>368111100</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6">
+    <row r="61" spans="1:12" ht="15.6">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
@@ -3739,17 +3919,20 @@
       <c r="H61">
         <v>178.36920000000001</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61">
+        <v>24.661384999999999</v>
+      </c>
+      <c r="J61" t="s">
         <v>196</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>306153050</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.6">
+    <row r="62" spans="1:12" ht="15.6">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
@@ -3775,17 +3958,20 @@
       <c r="H62">
         <v>215.95474999999999</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62">
+        <v>5.823213</v>
+      </c>
+      <c r="J62" t="s">
         <v>195</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>485136180</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.6">
+    <row r="63" spans="1:12" ht="15.6">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -3811,17 +3997,20 @@
       <c r="H63">
         <v>191.41318699999999</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63">
+        <v>4.6642749999999999</v>
+      </c>
+      <c r="J63" t="s">
         <v>195</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>449280384</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15.6">
+    <row r="64" spans="1:12" ht="15.6">
       <c r="A64" s="1" t="s">
         <v>66</v>
       </c>
@@ -3847,17 +4036,20 @@
       <c r="H64">
         <v>306.15550000000002</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64">
+        <v>7.1548749999999997</v>
+      </c>
+      <c r="J64" t="s">
         <v>195</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>444691772</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.6">
+    <row r="65" spans="1:12" ht="15.6">
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
@@ -3883,17 +4075,20 @@
       <c r="H65">
         <v>303.14766700000001</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65">
+        <v>7.5794170000000003</v>
+      </c>
+      <c r="J65" t="s">
         <v>195</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>269822568</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="15.6">
+    <row r="66" spans="1:12" ht="15.6">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
@@ -3919,17 +4114,20 @@
       <c r="H66">
         <v>338.52600000000001</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66">
+        <v>1.9034</v>
+      </c>
+      <c r="J66" t="s">
         <v>197</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>442894022</v>
       </c>
-      <c r="K66" t="s">
+      <c r="L66" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.6">
+    <row r="67" spans="1:12" ht="15.6">
       <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
@@ -3955,17 +4153,20 @@
       <c r="H67">
         <v>344.81234999999998</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67">
+        <v>0.73158999999999996</v>
+      </c>
+      <c r="J67" t="s">
         <v>197</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>402217188</v>
       </c>
-      <c r="K67" t="s">
+      <c r="L67" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.6">
+    <row r="68" spans="1:12" ht="15.6">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
@@ -3991,17 +4192,20 @@
       <c r="H68">
         <v>326.68029999999999</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I68">
+        <v>-0.79239499999999996</v>
+      </c>
+      <c r="J68" t="s">
         <v>197</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>437597746</v>
       </c>
-      <c r="K68" t="s">
+      <c r="L68" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15.6">
+    <row r="69" spans="1:12" ht="15.6">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
@@ -4027,17 +4231,20 @@
       <c r="H69">
         <v>203.7715</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69">
+        <v>0.45676299999999997</v>
+      </c>
+      <c r="J69" t="s">
         <v>197</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>408885864</v>
       </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.6">
+    <row r="70" spans="1:12" ht="15.6">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
@@ -4063,17 +4270,20 @@
       <c r="H70">
         <v>203.37975</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70">
+        <v>23.889250000000001</v>
+      </c>
+      <c r="J70" t="s">
         <v>196</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>338549582</v>
       </c>
-      <c r="K70" t="s">
+      <c r="L70" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15.6">
+    <row r="71" spans="1:12" ht="15.6">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
@@ -4099,17 +4309,20 @@
       <c r="H71">
         <v>204.42099999999999</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I71">
+        <v>24.958884999999999</v>
+      </c>
+      <c r="J71" t="s">
         <v>196</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>338697124</v>
       </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.6">
+    <row r="72" spans="1:12" ht="15.6">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
@@ -4135,17 +4348,20 @@
       <c r="H72">
         <v>104.99679999999999</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72">
+        <v>19.781234999999999</v>
+      </c>
+      <c r="J72" t="s">
         <v>196</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>409640862</v>
       </c>
-      <c r="K72" t="s">
+      <c r="L72" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.6">
+    <row r="73" spans="1:12" ht="15.6">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
@@ -4171,17 +4387,20 @@
       <c r="H73">
         <v>199.69110000000001</v>
       </c>
-      <c r="I73" t="s">
+      <c r="I73">
+        <v>27.497475000000001</v>
+      </c>
+      <c r="J73" t="s">
         <v>198</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>375963270</v>
       </c>
-      <c r="K73" t="s">
+      <c r="L73" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15.6">
+    <row r="74" spans="1:12" ht="15.6">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
@@ -4207,17 +4426,20 @@
       <c r="H74">
         <v>199.83029999999999</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74">
+        <v>26.019185</v>
+      </c>
+      <c r="J74" t="s">
         <v>198</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>340470354</v>
       </c>
-      <c r="K74" t="s">
+      <c r="L74" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15.6">
+    <row r="75" spans="1:12" ht="15.6">
       <c r="A75" s="1" t="s">
         <v>77</v>
       </c>
@@ -4243,17 +4465,20 @@
       <c r="H75">
         <v>2.2645620000000002</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75">
+        <v>11.142362</v>
+      </c>
+      <c r="J75" t="s">
         <v>198</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <v>388403914</v>
       </c>
-      <c r="K75" t="s">
+      <c r="L75" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15.6">
+    <row r="76" spans="1:12" ht="15.6">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
@@ -4279,17 +4504,20 @@
       <c r="H76">
         <v>201.67019999999999</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76">
+        <v>24.262869999999999</v>
+      </c>
+      <c r="J76" t="s">
         <v>196</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <v>399008374</v>
       </c>
-      <c r="K76" t="s">
+      <c r="L76" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15.6">
+    <row r="77" spans="1:12" ht="15.6">
       <c r="A77" s="1" t="s">
         <v>79</v>
       </c>
@@ -4315,17 +4543,20 @@
       <c r="H77">
         <v>206.43459999999999</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77">
+        <v>21.949369999999998</v>
+      </c>
+      <c r="J77" t="s">
         <v>196</v>
       </c>
-      <c r="J77">
+      <c r="K77">
         <v>412959348</v>
       </c>
-      <c r="K77" t="s">
+      <c r="L77" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="15.6">
+    <row r="78" spans="1:12" ht="15.6">
       <c r="A78" s="1" t="s">
         <v>80</v>
       </c>
@@ -4351,17 +4582,20 @@
       <c r="H78">
         <v>200.47062500000001</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78">
+        <v>5.7491060000000003</v>
+      </c>
+      <c r="J78" t="s">
         <v>196</v>
       </c>
-      <c r="J78">
+      <c r="K78">
         <v>303174866</v>
       </c>
-      <c r="K78" t="s">
+      <c r="L78" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15.6">
+    <row r="79" spans="1:12" ht="15.6">
       <c r="A79" s="1" t="s">
         <v>81</v>
       </c>
@@ -4387,17 +4621,20 @@
       <c r="H79">
         <v>5.1479999999999997</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79">
+        <v>9.1374379999999995</v>
+      </c>
+      <c r="J79" t="s">
         <v>196</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>399549740</v>
       </c>
-      <c r="K79" t="s">
+      <c r="L79" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.6">
+    <row r="80" spans="1:12" ht="15.6">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
@@ -4423,17 +4660,20 @@
       <c r="H80">
         <v>3.4942000000000002</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80">
+        <v>12.806365</v>
+      </c>
+      <c r="J80" t="s">
         <v>196</v>
       </c>
-      <c r="J80">
+      <c r="K80">
         <v>368875202</v>
       </c>
-      <c r="K80" t="s">
+      <c r="L80" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15.6">
+    <row r="81" spans="1:12" ht="15.6">
       <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
@@ -4459,17 +4699,20 @@
       <c r="H81">
         <v>201.01089999999999</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81">
+        <v>25.349495000000001</v>
+      </c>
+      <c r="J81" t="s">
         <v>196</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>373700996</v>
       </c>
-      <c r="K81" t="s">
+      <c r="L81" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15.6">
+    <row r="82" spans="1:12" ht="15.6">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
@@ -4495,17 +4738,20 @@
       <c r="H82">
         <v>216.67805000000001</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I82">
+        <v>22.596675000000001</v>
+      </c>
+      <c r="J82" t="s">
         <v>196</v>
       </c>
-      <c r="J82">
+      <c r="K82">
         <v>341739196</v>
       </c>
-      <c r="K82" t="s">
+      <c r="L82" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15.6">
+    <row r="83" spans="1:12" ht="15.6">
       <c r="A83" s="1" t="s">
         <v>85</v>
       </c>
@@ -4531,17 +4777,20 @@
       <c r="H83">
         <v>204.54175000000001</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83">
+        <v>23.845330000000001</v>
+      </c>
+      <c r="J83" t="s">
         <v>196</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>377820080</v>
       </c>
-      <c r="K83" t="s">
+      <c r="L83" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15.6">
+    <row r="84" spans="1:12" ht="15.6">
       <c r="A84" s="1" t="s">
         <v>86</v>
       </c>
@@ -4567,17 +4816,20 @@
       <c r="H84">
         <v>154.67009999999999</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84">
+        <v>7.9683700000000002</v>
+      </c>
+      <c r="J84" t="s">
         <v>196</v>
       </c>
-      <c r="J84">
+      <c r="K84">
         <v>451528640</v>
       </c>
-      <c r="K84" t="s">
+      <c r="L84" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15.6">
+    <row r="85" spans="1:12" ht="15.6">
       <c r="A85" s="1" t="s">
         <v>87</v>
       </c>
@@ -4603,17 +4855,20 @@
       <c r="H85">
         <v>200.40835000000001</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85">
+        <v>25.18103</v>
+      </c>
+      <c r="J85" t="s">
         <v>196</v>
       </c>
-      <c r="J85">
+      <c r="K85">
         <v>253952482</v>
       </c>
-      <c r="K85" t="s">
+      <c r="L85" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="15.6">
+    <row r="86" spans="1:12" ht="15.6">
       <c r="A86" s="1" t="s">
         <v>88</v>
       </c>
@@ -4639,17 +4894,20 @@
       <c r="H86">
         <v>208.821</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86">
+        <v>20.212700000000002</v>
+      </c>
+      <c r="J86" t="s">
         <v>196</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>256287760</v>
       </c>
-      <c r="K86" t="s">
+      <c r="L86" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15.6">
+    <row r="87" spans="1:12" ht="15.6">
       <c r="A87" s="1" t="s">
         <v>89</v>
       </c>
@@ -4675,17 +4933,20 @@
       <c r="H87">
         <v>219.01499999999999</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87">
+        <v>21.121575</v>
+      </c>
+      <c r="J87" t="s">
         <v>196</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>460018862</v>
       </c>
-      <c r="K87" t="s">
+      <c r="L87" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15.6">
+    <row r="88" spans="1:12" ht="15.6">
       <c r="A88" s="1" t="s">
         <v>90</v>
       </c>
@@ -4711,17 +4972,20 @@
       <c r="H88">
         <v>227.76089999999999</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I88">
+        <v>15.376875</v>
+      </c>
+      <c r="J88" t="s">
         <v>196</v>
       </c>
-      <c r="J88">
+      <c r="K88">
         <v>338611726</v>
       </c>
-      <c r="K88" t="s">
+      <c r="L88" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15.6">
+    <row r="89" spans="1:12" ht="15.6">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -4747,17 +5011,20 @@
       <c r="H89">
         <v>243.04079999999999</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89">
+        <v>18.122955000000001</v>
+      </c>
+      <c r="J89" t="s">
         <v>196</v>
       </c>
-      <c r="J89">
+      <c r="K89">
         <v>274983484</v>
       </c>
-      <c r="K89" t="s">
+      <c r="L89" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15.6">
+    <row r="90" spans="1:12" ht="15.6">
       <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
@@ -4783,17 +5050,20 @@
       <c r="H90">
         <v>2.4397500000000001</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I90">
+        <v>10.082375000000001</v>
+      </c>
+      <c r="J90" t="s">
         <v>196</v>
       </c>
-      <c r="J90">
+      <c r="K90">
         <v>385005800</v>
       </c>
-      <c r="K90" t="s">
+      <c r="L90" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15.6">
+    <row r="91" spans="1:12" ht="15.6">
       <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
@@ -4819,17 +5089,20 @@
       <c r="H91">
         <v>223.15899999999999</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91">
+        <v>19.24802</v>
+      </c>
+      <c r="J91" t="s">
         <v>198</v>
       </c>
-      <c r="J91">
+      <c r="K91">
         <v>539113764</v>
       </c>
-      <c r="K91" t="s">
+      <c r="L91" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15.6">
+    <row r="92" spans="1:12" ht="15.6">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -4855,17 +5128,20 @@
       <c r="H92">
         <v>236.1591</v>
       </c>
-      <c r="I92" t="s">
+      <c r="I92">
+        <v>13.874504999999999</v>
+      </c>
+      <c r="J92" t="s">
         <v>198</v>
       </c>
-      <c r="J92">
+      <c r="K92">
         <v>359284260</v>
       </c>
-      <c r="K92" t="s">
+      <c r="L92" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15.6">
+    <row r="93" spans="1:12" ht="15.6">
       <c r="A93" s="1" t="s">
         <v>95</v>
       </c>
@@ -4891,17 +5167,20 @@
       <c r="H93">
         <v>9.4647500000000004</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93">
+        <v>4.9188749999999999</v>
+      </c>
+      <c r="J93" t="s">
         <v>198</v>
       </c>
-      <c r="J93">
+      <c r="K93">
         <v>437816192</v>
       </c>
-      <c r="K93" t="s">
+      <c r="L93" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15.6">
+    <row r="94" spans="1:12" ht="15.6">
       <c r="A94" s="1" t="s">
         <v>96</v>
       </c>
@@ -4927,17 +5206,20 @@
       <c r="H94">
         <v>191.91255000000001</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94">
+        <v>23.888159999999999</v>
+      </c>
+      <c r="J94" t="s">
         <v>196</v>
       </c>
-      <c r="J94">
+      <c r="K94">
         <v>321797088</v>
       </c>
-      <c r="K94" t="s">
+      <c r="L94" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15.6">
+    <row r="95" spans="1:12" ht="15.6">
       <c r="A95" s="1" t="s">
         <v>97</v>
       </c>
@@ -4963,17 +5245,20 @@
       <c r="H95">
         <v>145.08179999999999</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I95">
+        <v>22.039784999999998</v>
+      </c>
+      <c r="J95" t="s">
         <v>196</v>
       </c>
-      <c r="J95">
+      <c r="K95">
         <v>423500782</v>
       </c>
-      <c r="K95" t="s">
+      <c r="L95" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="15.6">
+    <row r="96" spans="1:12" ht="15.6">
       <c r="A96" s="1" t="s">
         <v>98</v>
       </c>
@@ -4999,17 +5284,20 @@
       <c r="H96">
         <v>187.07695000000001</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96">
+        <v>26.604669999999999</v>
+      </c>
+      <c r="J96" t="s">
         <v>196</v>
       </c>
-      <c r="J96">
+      <c r="K96">
         <v>278380318</v>
       </c>
-      <c r="K96" t="s">
+      <c r="L96" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15.6">
+    <row r="97" spans="1:12" ht="15.6">
       <c r="A97" s="1" t="s">
         <v>99</v>
       </c>
@@ -5035,17 +5323,20 @@
       <c r="H97">
         <v>187.3321</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97">
+        <v>26.806039999999999</v>
+      </c>
+      <c r="J97" t="s">
         <v>196</v>
       </c>
-      <c r="J97">
+      <c r="K97">
         <v>328505148</v>
       </c>
-      <c r="K97" t="s">
+      <c r="L97" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="15.6">
+    <row r="98" spans="1:12" ht="15.6">
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
@@ -5071,17 +5362,20 @@
       <c r="H98">
         <v>160.81444999999999</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98">
+        <v>23.681605000000001</v>
+      </c>
+      <c r="J98" t="s">
         <v>196</v>
       </c>
-      <c r="J98">
+      <c r="K98">
         <v>370803024</v>
       </c>
-      <c r="K98" t="s">
+      <c r="L98" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15.6">
+    <row r="99" spans="1:12" ht="15.6">
       <c r="A99" s="1" t="s">
         <v>101</v>
       </c>
@@ -5107,17 +5401,20 @@
       <c r="H99">
         <v>236.78925000000001</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99">
+        <v>13.993715</v>
+      </c>
+      <c r="J99" t="s">
         <v>199</v>
       </c>
-      <c r="J99">
+      <c r="K99">
         <v>352030928</v>
       </c>
-      <c r="K99" t="s">
+      <c r="L99" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15.6">
+    <row r="100" spans="1:12" ht="15.6">
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
@@ -5143,17 +5440,20 @@
       <c r="H100">
         <v>232.660562</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100">
+        <v>5.0041690000000001</v>
+      </c>
+      <c r="J100" t="s">
         <v>199</v>
       </c>
-      <c r="J100">
+      <c r="K100">
         <v>354224626</v>
       </c>
-      <c r="K100" t="s">
+      <c r="L100" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="15.6">
+    <row r="101" spans="1:12" ht="15.6">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
@@ -5179,17 +5479,20 @@
       <c r="H101">
         <v>137.33439999999999</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101">
+        <v>10.685499999999999</v>
+      </c>
+      <c r="J101" t="s">
         <v>199</v>
       </c>
-      <c r="J101">
+      <c r="K101">
         <v>307846576</v>
       </c>
-      <c r="K101" t="s">
+      <c r="L101" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="15.6">
+    <row r="102" spans="1:12" ht="15.6">
       <c r="A102" s="1" t="s">
         <v>104</v>
       </c>
@@ -5215,17 +5518,20 @@
       <c r="H102">
         <v>242.84049999999999</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102">
+        <v>14.316750000000001</v>
+      </c>
+      <c r="J102" t="s">
         <v>199</v>
       </c>
-      <c r="J102">
+      <c r="K102">
         <v>329240054</v>
       </c>
-      <c r="K102" t="s">
+      <c r="L102" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="15.6">
+    <row r="103" spans="1:12" ht="15.6">
       <c r="A103" s="1" t="s">
         <v>105</v>
       </c>
@@ -5251,17 +5557,20 @@
       <c r="H103">
         <v>241.15729999999999</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103">
+        <v>14.29128</v>
+      </c>
+      <c r="J103" t="s">
         <v>199</v>
       </c>
-      <c r="J103">
+      <c r="K103">
         <v>388462874</v>
       </c>
-      <c r="K103" t="s">
+      <c r="L103" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="15.6">
+    <row r="104" spans="1:12" ht="15.6">
       <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
@@ -5287,17 +5596,20 @@
       <c r="H104">
         <v>174.85133300000001</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I104">
+        <v>10.167674999999999</v>
+      </c>
+      <c r="J104" t="s">
         <v>199</v>
       </c>
-      <c r="J104">
+      <c r="K104">
         <v>345574560</v>
       </c>
-      <c r="K104" t="s">
+      <c r="L104" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15.6">
+    <row r="105" spans="1:12" ht="15.6">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
@@ -5323,17 +5635,20 @@
       <c r="H105">
         <v>131.97941700000001</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105">
+        <v>6.6343920000000001</v>
+      </c>
+      <c r="J105" t="s">
         <v>198</v>
       </c>
-      <c r="J105">
+      <c r="K105">
         <v>407894524</v>
       </c>
-      <c r="K105" t="s">
+      <c r="L105" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="15.6">
+    <row r="106" spans="1:12" ht="15.6">
       <c r="A106" s="1" t="s">
         <v>108</v>
       </c>
@@ -5359,17 +5674,20 @@
       <c r="H106">
         <v>197.72450000000001</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106">
+        <v>25.164594999999998</v>
+      </c>
+      <c r="J106" t="s">
         <v>198</v>
       </c>
-      <c r="J106">
+      <c r="K106">
         <v>333427578</v>
       </c>
-      <c r="K106" t="s">
+      <c r="L106" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15.6">
+    <row r="107" spans="1:12" ht="15.6">
       <c r="A107" s="1" t="s">
         <v>109</v>
       </c>
@@ -5395,17 +5713,20 @@
       <c r="H107">
         <v>222.94125</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107">
+        <v>15.321075</v>
+      </c>
+      <c r="J107" t="s">
         <v>198</v>
       </c>
-      <c r="J107">
+      <c r="K107">
         <v>522620482</v>
       </c>
-      <c r="K107" t="s">
+      <c r="L107" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="15.6">
+    <row r="108" spans="1:12" ht="15.6">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
@@ -5431,17 +5752,20 @@
       <c r="H108">
         <v>195.77195</v>
       </c>
-      <c r="I108" t="s">
+      <c r="I108">
+        <v>26.478605000000002</v>
+      </c>
+      <c r="J108" t="s">
         <v>198</v>
       </c>
-      <c r="J108">
+      <c r="K108">
         <v>371142378</v>
       </c>
-      <c r="K108" t="s">
+      <c r="L108" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="15.6">
+    <row r="109" spans="1:12" ht="15.6">
       <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
@@ -5467,17 +5791,20 @@
       <c r="H109">
         <v>213.96350000000001</v>
       </c>
-      <c r="I109" t="s">
+      <c r="I109">
+        <v>19.312774999999998</v>
+      </c>
+      <c r="J109" t="s">
         <v>199</v>
       </c>
-      <c r="J109">
+      <c r="K109">
         <v>338943134</v>
       </c>
-      <c r="K109" t="s">
+      <c r="L109" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="15.6">
+    <row r="110" spans="1:12" ht="15.6">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
@@ -5503,17 +5830,20 @@
       <c r="H110">
         <v>228.11654999999999</v>
       </c>
-      <c r="I110" t="s">
+      <c r="I110">
+        <v>16.747029999999999</v>
+      </c>
+      <c r="J110" t="s">
         <v>199</v>
       </c>
-      <c r="J110">
+      <c r="K110">
         <v>369538288</v>
       </c>
-      <c r="K110" t="s">
+      <c r="L110" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15.6">
+    <row r="111" spans="1:12" ht="15.6">
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
@@ -5539,17 +5869,20 @@
       <c r="H111">
         <v>232.28725</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I111">
+        <v>17.303004999999999</v>
+      </c>
+      <c r="J111" t="s">
         <v>199</v>
       </c>
-      <c r="J111">
+      <c r="K111">
         <v>396286730</v>
       </c>
-      <c r="K111" t="s">
+      <c r="L111" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15.6">
+    <row r="112" spans="1:12" ht="15.6">
       <c r="A112" s="1" t="s">
         <v>114</v>
       </c>
@@ -5575,17 +5908,20 @@
       <c r="H112">
         <v>213.68889999999999</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I112">
+        <v>20.481195</v>
+      </c>
+      <c r="J112" t="s">
         <v>199</v>
       </c>
-      <c r="J112">
+      <c r="K112">
         <v>346238396</v>
       </c>
-      <c r="K112" t="s">
+      <c r="L112" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15.6">
+    <row r="113" spans="1:12" ht="15.6">
       <c r="A113" s="1" t="s">
         <v>115</v>
       </c>
@@ -5611,17 +5947,20 @@
       <c r="H113">
         <v>192.24618699999999</v>
       </c>
-      <c r="I113" t="s">
+      <c r="I113">
+        <v>18.129193999999998</v>
+      </c>
+      <c r="J113" t="s">
         <v>199</v>
       </c>
-      <c r="J113">
+      <c r="K113">
         <v>339721848</v>
       </c>
-      <c r="K113" t="s">
+      <c r="L113" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="15.6">
+    <row r="114" spans="1:12" ht="15.6">
       <c r="A114" s="1" t="s">
         <v>116</v>
       </c>
@@ -5647,17 +5986,20 @@
       <c r="H114">
         <v>220.94919999999999</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I114">
+        <v>18.82554</v>
+      </c>
+      <c r="J114" t="s">
         <v>199</v>
       </c>
-      <c r="J114">
+      <c r="K114">
         <v>357891876</v>
       </c>
-      <c r="K114" t="s">
+      <c r="L114" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15.6">
+    <row r="115" spans="1:12" ht="15.6">
       <c r="A115" s="1" t="s">
         <v>117</v>
       </c>
@@ -5683,17 +6025,20 @@
       <c r="H115">
         <v>152.71950000000001</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I115">
+        <v>10.496305</v>
+      </c>
+      <c r="J115" t="s">
         <v>199</v>
       </c>
-      <c r="J115">
+      <c r="K115">
         <v>388065794</v>
       </c>
-      <c r="K115" t="s">
+      <c r="L115" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="15.6">
+    <row r="116" spans="1:12" ht="15.6">
       <c r="A116" s="1" t="s">
         <v>118</v>
       </c>
@@ -5719,17 +6064,20 @@
       <c r="H116">
         <v>229.36808300000001</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I116">
+        <v>17.627141999999999</v>
+      </c>
+      <c r="J116" t="s">
         <v>199</v>
       </c>
-      <c r="J116">
+      <c r="K116">
         <v>387769558</v>
       </c>
-      <c r="K116" t="s">
+      <c r="L116" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="15.6">
+    <row r="117" spans="1:12" ht="15.6">
       <c r="A117" s="1" t="s">
         <v>119</v>
       </c>
@@ -5755,17 +6103,20 @@
       <c r="H117">
         <v>229.097917</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I117">
+        <v>17.585567000000001</v>
+      </c>
+      <c r="J117" t="s">
         <v>199</v>
       </c>
-      <c r="J117">
+      <c r="K117">
         <v>364054734</v>
       </c>
-      <c r="K117" t="s">
+      <c r="L117" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="15.6">
+    <row r="118" spans="1:12" ht="15.6">
       <c r="A118" s="1" t="s">
         <v>120</v>
       </c>
@@ -5791,17 +6142,20 @@
       <c r="H118">
         <v>195.50287499999999</v>
       </c>
-      <c r="I118" t="s">
+      <c r="I118">
+        <v>27.167300000000001</v>
+      </c>
+      <c r="J118" t="s">
         <v>199</v>
       </c>
-      <c r="J118">
+      <c r="K118">
         <v>342398030</v>
       </c>
-      <c r="K118" t="s">
+      <c r="L118" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15.6">
+    <row r="119" spans="1:12" ht="15.6">
       <c r="A119" s="1" t="s">
         <v>121</v>
       </c>
@@ -5827,17 +6181,20 @@
       <c r="H119">
         <v>123.20099999999999</v>
       </c>
-      <c r="I119" t="s">
+      <c r="I119">
+        <v>20.585740000000001</v>
+      </c>
+      <c r="J119" t="s">
         <v>198</v>
       </c>
-      <c r="J119">
+      <c r="K119">
         <v>385071042</v>
       </c>
-      <c r="K119" t="s">
+      <c r="L119" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="15.6">
+    <row r="120" spans="1:12" ht="15.6">
       <c r="A120" s="1" t="s">
         <v>122</v>
       </c>
@@ -5863,17 +6220,20 @@
       <c r="H120">
         <v>0.83231299999999997</v>
       </c>
-      <c r="I120" t="s">
+      <c r="I120">
+        <v>8.8871310000000001</v>
+      </c>
+      <c r="J120" t="s">
         <v>198</v>
       </c>
-      <c r="J120">
+      <c r="K120">
         <v>402714396</v>
       </c>
-      <c r="K120" t="s">
+      <c r="L120" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15.6">
+    <row r="121" spans="1:12" ht="15.6">
       <c r="A121" s="1" t="s">
         <v>123</v>
       </c>
@@ -5899,17 +6259,20 @@
       <c r="H121">
         <v>196.2029</v>
       </c>
-      <c r="I121" t="s">
+      <c r="I121">
+        <v>26.605515</v>
+      </c>
+      <c r="J121" t="s">
         <v>198</v>
       </c>
-      <c r="J121">
+      <c r="K121">
         <v>342278366</v>
       </c>
-      <c r="K121" t="s">
+      <c r="L121" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="15.6">
+    <row r="122" spans="1:12" ht="15.6">
       <c r="A122" s="1" t="s">
         <v>124</v>
       </c>
@@ -5935,17 +6298,20 @@
       <c r="H122">
         <v>41.525149999999996</v>
       </c>
-      <c r="I122" t="s">
+      <c r="I122">
+        <v>17.291965000000001</v>
+      </c>
+      <c r="J122" t="s">
         <v>198</v>
       </c>
-      <c r="J122">
+      <c r="K122">
         <v>391822972</v>
       </c>
-      <c r="K122" t="s">
+      <c r="L122" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15.6">
+    <row r="123" spans="1:12" ht="15.6">
       <c r="A123" s="1" t="s">
         <v>125</v>
       </c>
@@ -5971,17 +6337,20 @@
       <c r="H123">
         <v>1.0133129999999999</v>
       </c>
-      <c r="I123" t="s">
+      <c r="I123">
+        <v>8.1498939999999997</v>
+      </c>
+      <c r="J123" t="s">
         <v>198</v>
       </c>
-      <c r="J123">
+      <c r="K123">
         <v>346225714</v>
       </c>
-      <c r="K123" t="s">
+      <c r="L123" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15.6">
+    <row r="124" spans="1:12" ht="15.6">
       <c r="A124" s="1" t="s">
         <v>126</v>
       </c>
@@ -6007,17 +6376,20 @@
       <c r="H124">
         <v>205.411</v>
       </c>
-      <c r="I124" t="s">
+      <c r="I124">
+        <v>26.555662999999999</v>
+      </c>
+      <c r="J124" t="s">
         <v>198</v>
       </c>
-      <c r="J124">
+      <c r="K124">
         <v>370334582</v>
       </c>
-      <c r="K124" t="s">
+      <c r="L124" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="15.6">
+    <row r="125" spans="1:12" ht="15.6">
       <c r="A125" s="1" t="s">
         <v>127</v>
       </c>
@@ -6043,17 +6415,20 @@
       <c r="H125">
         <v>108.231313</v>
       </c>
-      <c r="I125" t="s">
+      <c r="I125">
+        <v>9.7350750000000001</v>
+      </c>
+      <c r="J125" t="s">
         <v>199</v>
       </c>
-      <c r="J125">
+      <c r="K125">
         <v>328237008</v>
       </c>
-      <c r="K125" t="s">
+      <c r="L125" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="15.6">
+    <row r="126" spans="1:12" ht="15.6">
       <c r="A126" s="1" t="s">
         <v>128</v>
       </c>
@@ -6079,17 +6454,20 @@
       <c r="H126">
         <v>195.54124999999999</v>
       </c>
-      <c r="I126" t="s">
+      <c r="I126">
+        <v>24.984559999999998</v>
+      </c>
+      <c r="J126" t="s">
         <v>199</v>
       </c>
-      <c r="J126">
+      <c r="K126">
         <v>314283624</v>
       </c>
-      <c r="K126" t="s">
+      <c r="L126" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="15.6">
+    <row r="127" spans="1:12" ht="15.6">
       <c r="A127" s="1" t="s">
         <v>129</v>
       </c>
@@ -6115,17 +6493,20 @@
       <c r="H127">
         <v>193.38225</v>
       </c>
-      <c r="I127" t="s">
+      <c r="I127">
+        <v>24.961604999999999</v>
+      </c>
+      <c r="J127" t="s">
         <v>199</v>
       </c>
-      <c r="J127">
+      <c r="K127">
         <v>311581824</v>
       </c>
-      <c r="K127" t="s">
+      <c r="L127" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="15.6">
+    <row r="128" spans="1:12" ht="15.6">
       <c r="A128" s="1" t="s">
         <v>130</v>
       </c>
@@ -6151,17 +6532,20 @@
       <c r="H128">
         <v>271.06412499999999</v>
       </c>
-      <c r="I128" t="s">
+      <c r="I128">
+        <v>11.095470000000001</v>
+      </c>
+      <c r="J128" t="s">
         <v>199</v>
       </c>
-      <c r="J128">
+      <c r="K128">
         <v>397681922</v>
       </c>
-      <c r="K128" t="s">
+      <c r="L128" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15.6">
+    <row r="129" spans="1:12" ht="15.6">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -6187,17 +6571,20 @@
       <c r="H129">
         <v>266.47312499999998</v>
       </c>
-      <c r="I129" t="s">
+      <c r="I129">
+        <v>10.790179999999999</v>
+      </c>
+      <c r="J129" t="s">
         <v>199</v>
       </c>
-      <c r="J129">
+      <c r="K129">
         <v>357393502</v>
       </c>
-      <c r="K129" t="s">
+      <c r="L129" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="15.6">
+    <row r="130" spans="1:12" ht="15.6">
       <c r="A130" s="1" t="s">
         <v>132</v>
       </c>
@@ -6223,17 +6610,20 @@
       <c r="H130">
         <v>208.76175000000001</v>
       </c>
-      <c r="I130" t="s">
+      <c r="I130">
+        <v>8.9235810000000004</v>
+      </c>
+      <c r="J130" t="s">
         <v>199</v>
       </c>
-      <c r="J130">
+      <c r="K130">
         <v>370391086</v>
       </c>
-      <c r="K130" t="s">
+      <c r="L130" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="15.6">
+    <row r="131" spans="1:12" ht="15.6">
       <c r="A131" s="1" t="s">
         <v>133</v>
       </c>
@@ -6259,17 +6649,20 @@
       <c r="H131">
         <v>299.00729999999999</v>
       </c>
-      <c r="I131" t="s">
+      <c r="I131">
+        <v>7.48766</v>
+      </c>
+      <c r="J131" t="s">
         <v>200</v>
       </c>
-      <c r="J131">
+      <c r="K131">
         <v>281316518</v>
       </c>
-      <c r="K131" t="s">
+      <c r="L131" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="15.6">
+    <row r="132" spans="1:12" ht="15.6">
       <c r="A132" s="1" t="s">
         <v>134</v>
       </c>
@@ -6295,17 +6688,20 @@
       <c r="H132">
         <v>303.31905</v>
       </c>
-      <c r="I132" t="s">
+      <c r="I132">
+        <v>3.1072000000000002</v>
+      </c>
+      <c r="J132" t="s">
         <v>200</v>
       </c>
-      <c r="J132">
+      <c r="K132">
         <v>322501268</v>
       </c>
-      <c r="K132" t="s">
+      <c r="L132" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="15.6">
+    <row r="133" spans="1:12" ht="15.6">
       <c r="A133" s="1" t="s">
         <v>136</v>
       </c>
@@ -6331,17 +6727,20 @@
       <c r="H133">
         <v>326.36090000000002</v>
       </c>
-      <c r="I133" t="s">
+      <c r="I133">
+        <v>3.8245450000000001</v>
+      </c>
+      <c r="J133" t="s">
         <v>200</v>
       </c>
-      <c r="J133">
+      <c r="K133">
         <v>339465160</v>
       </c>
-      <c r="K133" t="s">
+      <c r="L133" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="15.6">
+    <row r="134" spans="1:12" ht="15.6">
       <c r="A134" s="1" t="s">
         <v>137</v>
       </c>
@@ -6367,17 +6766,20 @@
       <c r="H134">
         <v>385.28075000000001</v>
       </c>
-      <c r="I134" t="s">
+      <c r="I134">
+        <v>-0.16031200000000001</v>
+      </c>
+      <c r="J134" t="s">
         <v>200</v>
       </c>
-      <c r="J134">
+      <c r="K134">
         <v>342121874</v>
       </c>
-      <c r="K134" t="s">
+      <c r="L134" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="15.6">
+    <row r="135" spans="1:12" ht="15.6">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -6403,17 +6805,20 @@
       <c r="H135">
         <v>348.00062500000001</v>
       </c>
-      <c r="I135" t="s">
+      <c r="I135">
+        <v>-1.2978499999999999</v>
+      </c>
+      <c r="J135" t="s">
         <v>200</v>
       </c>
-      <c r="J135">
+      <c r="K135">
         <v>318044830</v>
       </c>
-      <c r="K135" t="s">
+      <c r="L135" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15.6">
+    <row r="136" spans="1:12" ht="15.6">
       <c r="A136" s="1" t="s">
         <v>139</v>
       </c>
@@ -6439,17 +6844,20 @@
       <c r="H136">
         <v>314.71674999999999</v>
       </c>
-      <c r="I136" t="s">
+      <c r="I136">
+        <v>1.0257050000000001</v>
+      </c>
+      <c r="J136" t="s">
         <v>200</v>
       </c>
-      <c r="J136">
+      <c r="K136">
         <v>263756272</v>
       </c>
-      <c r="K136" t="s">
+      <c r="L136" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="15.6">
+    <row r="137" spans="1:12" ht="15.6">
       <c r="A137" s="1" t="s">
         <v>140</v>
       </c>
@@ -6475,17 +6883,20 @@
       <c r="H137">
         <v>369.28981199999998</v>
       </c>
-      <c r="I137" t="s">
+      <c r="I137">
+        <v>1.3657049999999999</v>
+      </c>
+      <c r="J137" t="s">
         <v>200</v>
       </c>
-      <c r="J137">
+      <c r="K137">
         <v>351574504</v>
       </c>
-      <c r="K137" t="s">
+      <c r="L137" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15.6">
+    <row r="138" spans="1:12" ht="15.6">
       <c r="A138" s="1" t="s">
         <v>141</v>
       </c>
@@ -6511,17 +6922,20 @@
       <c r="H138">
         <v>296.22800000000001</v>
       </c>
-      <c r="I138" t="s">
+      <c r="I138">
+        <v>1.47689</v>
+      </c>
+      <c r="J138" t="s">
         <v>200</v>
       </c>
-      <c r="J138">
+      <c r="K138">
         <v>327623186</v>
       </c>
-      <c r="K138" t="s">
+      <c r="L138" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15.6">
+    <row r="139" spans="1:12" ht="15.6">
       <c r="A139" s="1" t="s">
         <v>142</v>
       </c>
@@ -6547,17 +6961,20 @@
       <c r="H139">
         <v>315.37205</v>
       </c>
-      <c r="I139" t="s">
+      <c r="I139">
+        <v>9.9534999999999998E-2</v>
+      </c>
+      <c r="J139" t="s">
         <v>200</v>
       </c>
-      <c r="J139">
+      <c r="K139">
         <v>440972758</v>
       </c>
-      <c r="K139" t="s">
+      <c r="L139" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15.6">
+    <row r="140" spans="1:12" ht="15.6">
       <c r="A140" s="1" t="s">
         <v>143</v>
       </c>
@@ -6583,17 +7000,20 @@
       <c r="H140">
         <v>348.19666699999999</v>
       </c>
-      <c r="I140" t="s">
+      <c r="I140">
+        <v>1.325833</v>
+      </c>
+      <c r="J140" t="s">
         <v>200</v>
       </c>
-      <c r="J140">
+      <c r="K140">
         <v>336511738</v>
       </c>
-      <c r="K140" t="s">
+      <c r="L140" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15.6">
+    <row r="141" spans="1:12" ht="15.6">
       <c r="A141" s="1" t="s">
         <v>144</v>
       </c>
@@ -6619,17 +7039,20 @@
       <c r="H141">
         <v>356.22391699999997</v>
       </c>
-      <c r="I141" t="s">
+      <c r="I141">
+        <v>-1.5334920000000001</v>
+      </c>
+      <c r="J141" t="s">
         <v>200</v>
       </c>
-      <c r="J141">
+      <c r="K141">
         <v>386120244</v>
       </c>
-      <c r="K141" t="s">
+      <c r="L141" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15.6">
+    <row r="142" spans="1:12" ht="15.6">
       <c r="A142" s="1" t="s">
         <v>145</v>
       </c>
@@ -6655,17 +7078,20 @@
       <c r="H142">
         <v>388.30387500000001</v>
       </c>
-      <c r="I142" t="s">
+      <c r="I142">
+        <v>-1.6497379999999999</v>
+      </c>
+      <c r="J142" t="s">
         <v>200</v>
       </c>
-      <c r="J142">
+      <c r="K142">
         <v>404391722</v>
       </c>
-      <c r="K142" t="s">
+      <c r="L142" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15.6">
+    <row r="143" spans="1:12" ht="15.6">
       <c r="A143" s="1" t="s">
         <v>146</v>
       </c>
@@ -6691,17 +7117,20 @@
       <c r="H143">
         <v>373.06099999999998</v>
       </c>
-      <c r="I143" t="s">
+      <c r="I143">
+        <v>-1.6472439999999999</v>
+      </c>
+      <c r="J143" t="s">
         <v>200</v>
       </c>
-      <c r="J143">
+      <c r="K143">
         <v>338171936</v>
       </c>
-      <c r="K143" t="s">
+      <c r="L143" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15.6">
+    <row r="144" spans="1:12" ht="15.6">
       <c r="A144" s="1" t="s">
         <v>147</v>
       </c>
@@ -6727,17 +7156,20 @@
       <c r="H144">
         <v>363.64850000000001</v>
       </c>
-      <c r="I144" t="s">
+      <c r="I144">
+        <v>0.10149</v>
+      </c>
+      <c r="J144" t="s">
         <v>200</v>
       </c>
-      <c r="J144">
+      <c r="K144">
         <v>324346516</v>
       </c>
-      <c r="K144" t="s">
+      <c r="L144" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="15.6">
+    <row r="145" spans="1:12" ht="15.6">
       <c r="A145" s="1" t="s">
         <v>148</v>
       </c>
@@ -6763,17 +7195,20 @@
       <c r="H145">
         <v>371.05844999999999</v>
       </c>
-      <c r="I145" t="s">
+      <c r="I145">
+        <v>-0.60712500000000003</v>
+      </c>
+      <c r="J145" t="s">
         <v>200</v>
       </c>
-      <c r="J145">
+      <c r="K145">
         <v>282805050</v>
       </c>
-      <c r="K145" t="s">
+      <c r="L145" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="15.6">
+    <row r="146" spans="1:12" ht="15.6">
       <c r="A146" s="1" t="s">
         <v>149</v>
       </c>
@@ -6799,17 +7234,20 @@
       <c r="H146">
         <v>293.88900000000001</v>
       </c>
-      <c r="I146" t="s">
+      <c r="I146">
+        <v>1.5940399999999999</v>
+      </c>
+      <c r="J146" t="s">
         <v>200</v>
       </c>
-      <c r="J146">
+      <c r="K146">
         <v>324132078</v>
       </c>
-      <c r="K146" t="s">
+      <c r="L146" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="15.6">
+    <row r="147" spans="1:12" ht="15.6">
       <c r="A147" s="1" t="s">
         <v>150</v>
       </c>
@@ -6835,17 +7273,20 @@
       <c r="H147">
         <v>340.44375000000002</v>
       </c>
-      <c r="I147" t="s">
+      <c r="I147">
+        <v>1.48885</v>
+      </c>
+      <c r="J147" t="s">
         <v>200</v>
       </c>
-      <c r="J147">
+      <c r="K147">
         <v>342014496</v>
       </c>
-      <c r="K147" t="s">
+      <c r="L147" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="15.6">
+    <row r="148" spans="1:12" ht="15.6">
       <c r="A148" s="1" t="s">
         <v>151</v>
       </c>
@@ -6871,17 +7312,20 @@
       <c r="H148">
         <v>336.04075</v>
       </c>
-      <c r="I148" t="s">
+      <c r="I148">
+        <v>2.5693999999999999</v>
+      </c>
+      <c r="J148" t="s">
         <v>200</v>
       </c>
-      <c r="J148">
+      <c r="K148">
         <v>359981962</v>
       </c>
-      <c r="K148" t="s">
+      <c r="L148" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="15.6">
+    <row r="149" spans="1:12" ht="15.6">
       <c r="A149" s="1" t="s">
         <v>152</v>
       </c>
@@ -6907,17 +7351,20 @@
       <c r="H149">
         <v>271.87439999999998</v>
       </c>
-      <c r="I149" t="s">
+      <c r="I149">
+        <v>4.7913949999999996</v>
+      </c>
+      <c r="J149" t="s">
         <v>200</v>
       </c>
-      <c r="J149">
+      <c r="K149">
         <v>323196296</v>
       </c>
-      <c r="K149" t="s">
+      <c r="L149" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="15.6">
+    <row r="150" spans="1:12" ht="15.6">
       <c r="A150" s="1" t="s">
         <v>153</v>
       </c>
@@ -6943,17 +7390,20 @@
       <c r="H150">
         <v>293.84674999999999</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I150">
+        <v>5.2952649999999997</v>
+      </c>
+      <c r="J150" t="s">
         <v>200</v>
       </c>
-      <c r="J150">
+      <c r="K150">
         <v>320960112</v>
       </c>
-      <c r="K150" t="s">
+      <c r="L150" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="15.6">
+    <row r="151" spans="1:12" ht="15.6">
       <c r="A151" s="1" t="s">
         <v>154</v>
       </c>
@@ -6979,17 +7429,20 @@
       <c r="H151">
         <v>323.90156300000001</v>
       </c>
-      <c r="I151" t="s">
+      <c r="I151">
+        <v>2.4961250000000001</v>
+      </c>
+      <c r="J151" t="s">
         <v>200</v>
       </c>
-      <c r="J151">
+      <c r="K151">
         <v>295539040</v>
       </c>
-      <c r="K151" t="s">
+      <c r="L151" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="15.6">
+    <row r="152" spans="1:12" ht="15.6">
       <c r="A152" s="1" t="s">
         <v>155</v>
       </c>
@@ -7015,17 +7468,20 @@
       <c r="H152">
         <v>273.02834999999999</v>
       </c>
-      <c r="I152" t="s">
+      <c r="I152">
+        <v>4.2017300000000004</v>
+      </c>
+      <c r="J152" t="s">
         <v>200</v>
       </c>
-      <c r="J152">
+      <c r="K152">
         <v>321829274</v>
       </c>
-      <c r="K152" t="s">
+      <c r="L152" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="15.6">
+    <row r="153" spans="1:12" ht="15.6">
       <c r="A153" s="1" t="s">
         <v>156</v>
       </c>
@@ -7051,17 +7507,20 @@
       <c r="H153">
         <v>328.54665</v>
       </c>
-      <c r="I153" t="s">
+      <c r="I153">
+        <v>1.4453149999999999</v>
+      </c>
+      <c r="J153" t="s">
         <v>200</v>
       </c>
-      <c r="J153">
+      <c r="K153">
         <v>351923732</v>
       </c>
-      <c r="K153" t="s">
+      <c r="L153" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="15.6">
+    <row r="154" spans="1:12" ht="15.6">
       <c r="A154" s="1" t="s">
         <v>157</v>
       </c>
@@ -7087,17 +7546,20 @@
       <c r="H154">
         <v>230.08609999999999</v>
       </c>
-      <c r="I154" t="s">
+      <c r="I154">
+        <v>3.0355400000000001</v>
+      </c>
+      <c r="J154" t="s">
         <v>200</v>
       </c>
-      <c r="J154">
+      <c r="K154">
         <v>387847764</v>
       </c>
-      <c r="K154" t="s">
+      <c r="L154" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="15.6">
+    <row r="155" spans="1:12" ht="15.6">
       <c r="A155" s="1" t="s">
         <v>158</v>
       </c>
@@ -7123,17 +7585,20 @@
       <c r="H155">
         <v>357.164917</v>
       </c>
-      <c r="I155" t="s">
+      <c r="I155">
+        <v>2.5078870000000002</v>
+      </c>
+      <c r="J155" t="s">
         <v>200</v>
       </c>
-      <c r="J155">
+      <c r="K155">
         <v>304256672</v>
       </c>
-      <c r="K155" t="s">
+      <c r="L155" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="15.6">
+    <row r="156" spans="1:12" ht="15.6">
       <c r="A156" s="1" t="s">
         <v>159</v>
       </c>
@@ -7159,17 +7624,20 @@
       <c r="H156">
         <v>303.32600000000002</v>
       </c>
-      <c r="I156" t="s">
+      <c r="I156">
+        <v>3.1964999999999999</v>
+      </c>
+      <c r="J156" t="s">
         <v>200</v>
       </c>
-      <c r="J156">
+      <c r="K156">
         <v>347699812</v>
       </c>
-      <c r="K156" t="s">
+      <c r="L156" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="15.6">
+    <row r="157" spans="1:12" ht="15.6">
       <c r="A157" s="1" t="s">
         <v>160</v>
       </c>
@@ -7195,17 +7663,20 @@
       <c r="H157">
         <v>353.19349999999997</v>
       </c>
-      <c r="I157" t="s">
+      <c r="I157">
+        <v>-0.47922500000000001</v>
+      </c>
+      <c r="J157" t="s">
         <v>200</v>
       </c>
-      <c r="J157">
+      <c r="K157">
         <v>388341000</v>
       </c>
-      <c r="K157" t="s">
+      <c r="L157" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="15.6">
+    <row r="158" spans="1:12" ht="15.6">
       <c r="A158" s="1" t="s">
         <v>161</v>
       </c>
@@ -7231,17 +7702,20 @@
       <c r="H158">
         <v>227.316</v>
       </c>
-      <c r="I158" t="s">
+      <c r="I158">
+        <v>1.230869</v>
+      </c>
+      <c r="J158" t="s">
         <v>200</v>
       </c>
-      <c r="J158">
+      <c r="K158">
         <v>361095072</v>
       </c>
-      <c r="K158" t="s">
+      <c r="L158" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="15.6">
+    <row r="159" spans="1:12" ht="15.6">
       <c r="A159" s="1" t="s">
         <v>162</v>
       </c>
@@ -7267,17 +7741,20 @@
       <c r="H159">
         <v>368.52474999999998</v>
       </c>
-      <c r="I159" t="s">
+      <c r="I159">
+        <v>-1.32986</v>
+      </c>
+      <c r="J159" t="s">
         <v>200</v>
       </c>
-      <c r="J159">
+      <c r="K159">
         <v>482084694</v>
       </c>
-      <c r="K159" t="s">
+      <c r="L159" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="15.6">
+    <row r="160" spans="1:12" ht="15.6">
       <c r="A160" s="1" t="s">
         <v>163</v>
       </c>
@@ -7303,17 +7780,20 @@
       <c r="H160">
         <v>343.87783300000001</v>
       </c>
-      <c r="I160" t="s">
+      <c r="I160">
+        <v>-0.409335</v>
+      </c>
+      <c r="J160" t="s">
         <v>200</v>
       </c>
-      <c r="J160">
+      <c r="K160">
         <v>410083042</v>
       </c>
-      <c r="K160" t="s">
+      <c r="L160" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="15.6">
+    <row r="161" spans="1:12" ht="15.6">
       <c r="A161" s="1" t="s">
         <v>164</v>
       </c>
@@ -7339,17 +7819,20 @@
       <c r="H161">
         <v>233.31399999999999</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I161">
+        <v>0.99402500000000005</v>
+      </c>
+      <c r="J161" t="s">
         <v>200</v>
       </c>
-      <c r="J161">
+      <c r="K161">
         <v>327742496</v>
       </c>
-      <c r="K161" t="s">
+      <c r="L161" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="15.6">
+    <row r="162" spans="1:12" ht="15.6">
       <c r="A162" s="1" t="s">
         <v>165</v>
       </c>
@@ -7375,17 +7858,20 @@
       <c r="H162">
         <v>396.84808299999997</v>
       </c>
-      <c r="I162" t="s">
+      <c r="I162">
+        <v>-0.98783299999999996</v>
+      </c>
+      <c r="J162" t="s">
         <v>200</v>
       </c>
-      <c r="J162">
+      <c r="K162">
         <v>403570132</v>
       </c>
-      <c r="K162" t="s">
+      <c r="L162" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15.6">
+    <row r="163" spans="1:12" ht="15.6">
       <c r="A163" s="1" t="s">
         <v>166</v>
       </c>
@@ -7411,17 +7897,20 @@
       <c r="H163">
         <v>368.66262499999999</v>
       </c>
-      <c r="I163" t="s">
+      <c r="I163">
+        <v>-0.58533299999999999</v>
+      </c>
+      <c r="J163" t="s">
         <v>200</v>
       </c>
-      <c r="J163">
+      <c r="K163">
         <v>419019388</v>
       </c>
-      <c r="K163" t="s">
+      <c r="L163" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="15.6">
+    <row r="164" spans="1:12" ht="15.6">
       <c r="A164" s="1" t="s">
         <v>167</v>
       </c>
@@ -7447,17 +7936,20 @@
       <c r="H164">
         <v>339.44749999999999</v>
       </c>
-      <c r="I164" t="s">
+      <c r="I164">
+        <v>2.4533999999999998</v>
+      </c>
+      <c r="J164" t="s">
         <v>200</v>
       </c>
-      <c r="J164">
+      <c r="K164">
         <v>324730830</v>
       </c>
-      <c r="K164" t="s">
+      <c r="L164" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15.6">
+    <row r="165" spans="1:12" ht="15.6">
       <c r="A165" s="1" t="s">
         <v>168</v>
       </c>
@@ -7483,17 +7975,20 @@
       <c r="H165">
         <v>311.78269999999998</v>
       </c>
-      <c r="I165" t="s">
+      <c r="I165">
+        <v>8.4744700000000002</v>
+      </c>
+      <c r="J165" t="s">
         <v>200</v>
       </c>
-      <c r="J165">
+      <c r="K165">
         <v>402932612</v>
       </c>
-      <c r="K165" t="s">
+      <c r="L165" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15.6">
+    <row r="166" spans="1:12" ht="15.6">
       <c r="A166" s="1" t="s">
         <v>169</v>
       </c>
@@ -7519,17 +8014,20 @@
       <c r="H166">
         <v>304.04730000000001</v>
       </c>
-      <c r="I166" t="s">
+      <c r="I166">
+        <v>6.73489</v>
+      </c>
+      <c r="J166" t="s">
         <v>200</v>
       </c>
-      <c r="J166">
+      <c r="K166">
         <v>304435280</v>
       </c>
-      <c r="K166" t="s">
+      <c r="L166" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15.6">
+    <row r="167" spans="1:12" ht="15.6">
       <c r="A167" s="1" t="s">
         <v>170</v>
       </c>
@@ -7555,17 +8053,20 @@
       <c r="H167">
         <v>295.31094999999999</v>
       </c>
-      <c r="I167" t="s">
+      <c r="I167">
+        <v>0.22498000000000001</v>
+      </c>
+      <c r="J167" t="s">
         <v>200</v>
       </c>
-      <c r="J167">
+      <c r="K167">
         <v>291324614</v>
       </c>
-      <c r="K167" t="s">
+      <c r="L167" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15.6">
+    <row r="168" spans="1:12" ht="15.6">
       <c r="A168" s="1" t="s">
         <v>171</v>
       </c>
@@ -7591,17 +8092,20 @@
       <c r="H168">
         <v>363.00081299999999</v>
       </c>
-      <c r="I168" t="s">
+      <c r="I168">
+        <v>1.8996120000000001</v>
+      </c>
+      <c r="J168" t="s">
         <v>200</v>
       </c>
-      <c r="J168">
+      <c r="K168">
         <v>324989054</v>
       </c>
-      <c r="K168" t="s">
+      <c r="L168" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15.6">
+    <row r="169" spans="1:12" ht="15.6">
       <c r="A169" s="1" t="s">
         <v>172</v>
       </c>
@@ -7627,17 +8131,20 @@
       <c r="H169">
         <v>221.782083</v>
       </c>
-      <c r="I169" t="s">
+      <c r="I169">
+        <v>17.211742000000001</v>
+      </c>
+      <c r="J169" t="s">
         <v>194</v>
       </c>
-      <c r="J169">
+      <c r="K169">
         <v>151825104</v>
       </c>
-      <c r="K169" t="s">
+      <c r="L169" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15.6">
+    <row r="170" spans="1:12" ht="15.6">
       <c r="A170" s="1" t="s">
         <v>173</v>
       </c>
@@ -7663,17 +8170,20 @@
       <c r="H170">
         <v>224.26441700000001</v>
       </c>
-      <c r="I170" t="s">
+      <c r="I170">
+        <v>15.180558</v>
+      </c>
+      <c r="J170" t="s">
         <v>194</v>
       </c>
-      <c r="J170">
+      <c r="K170">
         <v>149845934</v>
       </c>
-      <c r="K170" t="s">
+      <c r="L170" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15.6">
+    <row r="171" spans="1:12" ht="15.6">
       <c r="A171" s="1" t="s">
         <v>174</v>
       </c>
@@ -7699,17 +8209,20 @@
       <c r="H171">
         <v>217.809833</v>
       </c>
-      <c r="I171" t="s">
+      <c r="I171">
+        <v>18.319192000000001</v>
+      </c>
+      <c r="J171" t="s">
         <v>194</v>
       </c>
-      <c r="J171">
+      <c r="K171">
         <v>458295920</v>
       </c>
-      <c r="K171" t="s">
+      <c r="L171" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15.6">
+    <row r="172" spans="1:12" ht="15.6">
       <c r="A172" s="1" t="s">
         <v>175</v>
       </c>
@@ -7735,17 +8248,20 @@
       <c r="H172">
         <v>229.908917</v>
       </c>
-      <c r="I172" t="s">
+      <c r="I172">
+        <v>15.181967</v>
+      </c>
+      <c r="J172" t="s">
         <v>194</v>
       </c>
-      <c r="J172">
+      <c r="K172">
         <v>387230740</v>
       </c>
-      <c r="K172" t="s">
+      <c r="L172" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15.6">
+    <row r="173" spans="1:12" ht="15.6">
       <c r="A173" s="1" t="s">
         <v>176</v>
       </c>
@@ -7771,17 +8287,20 @@
       <c r="H173">
         <v>238.694625</v>
       </c>
-      <c r="I173" t="s">
+      <c r="I173">
+        <v>18.30575</v>
+      </c>
+      <c r="J173" t="s">
         <v>194</v>
       </c>
-      <c r="J173">
+      <c r="K173">
         <v>408427272</v>
       </c>
-      <c r="K173" t="s">
+      <c r="L173" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15.6">
+    <row r="174" spans="1:12" ht="15.6">
       <c r="A174" s="1" t="s">
         <v>177</v>
       </c>
@@ -7804,17 +8323,20 @@
         <f t="shared" si="2"/>
         <v>1.6020599913279623</v>
       </c>
-      <c r="I174" t="s">
+      <c r="I174">
+        <v>16.3584</v>
+      </c>
+      <c r="J174" t="s">
         <v>199</v>
       </c>
-      <c r="J174">
+      <c r="K174">
         <v>476921334</v>
       </c>
-      <c r="K174" t="s">
+      <c r="L174" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15.6">
+    <row r="175" spans="1:12" ht="15.6">
       <c r="A175" s="1" t="s">
         <v>178</v>
       </c>
@@ -7837,17 +8359,20 @@
         <f t="shared" si="2"/>
         <v>0.95424250943932487</v>
       </c>
-      <c r="I175" t="s">
+      <c r="I175">
+        <v>24.482800000000001</v>
+      </c>
+      <c r="J175" t="s">
         <v>194</v>
       </c>
-      <c r="J175">
+      <c r="K175">
         <v>489617426</v>
       </c>
-      <c r="K175" t="s">
+      <c r="L175" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15.6">
+    <row r="176" spans="1:12" ht="15.6">
       <c r="A176" s="1" t="s">
         <v>179</v>
       </c>
@@ -7870,17 +8395,20 @@
         <f t="shared" si="2"/>
         <v>1.7403626894942439</v>
       </c>
-      <c r="I176" t="s">
+      <c r="I176">
+        <v>15.970800000000001</v>
+      </c>
+      <c r="J176" t="s">
         <v>194</v>
       </c>
-      <c r="J176">
+      <c r="K176">
         <v>416553274</v>
       </c>
-      <c r="K176" t="s">
+      <c r="L176" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="15.6">
+    <row r="177" spans="1:12" ht="15.6">
       <c r="A177" s="1" t="s">
         <v>180</v>
       </c>
@@ -7906,17 +8434,20 @@
       <c r="H177">
         <v>209.80708300000001</v>
       </c>
-      <c r="I177" t="s">
+      <c r="I177">
+        <v>25.681369</v>
+      </c>
+      <c r="J177" t="s">
         <v>201</v>
       </c>
-      <c r="J177">
+      <c r="K177">
         <v>252063110</v>
       </c>
-      <c r="K177" t="s">
+      <c r="L177" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="15.6">
+    <row r="178" spans="1:12" ht="15.6">
       <c r="A178" s="1" t="s">
         <v>181</v>
       </c>
@@ -7942,17 +8473,20 @@
       <c r="H178">
         <v>3.12405</v>
       </c>
-      <c r="I178" t="s">
+      <c r="I178">
+        <v>15.553794999999999</v>
+      </c>
+      <c r="J178" t="s">
         <v>201</v>
       </c>
-      <c r="J178">
+      <c r="K178">
         <v>277574946</v>
       </c>
-      <c r="K178" t="s">
+      <c r="L178" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="15.6">
+    <row r="179" spans="1:12" ht="15.6">
       <c r="A179" s="1" t="s">
         <v>182</v>
       </c>
@@ -7978,17 +8512,20 @@
       <c r="H179">
         <v>187.73949999999999</v>
       </c>
-      <c r="I179" t="s">
+      <c r="I179">
+        <v>26.313594999999999</v>
+      </c>
+      <c r="J179" t="s">
         <v>201</v>
       </c>
-      <c r="J179">
+      <c r="K179">
         <v>262268056</v>
       </c>
-      <c r="K179" t="s">
+      <c r="L179" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="15.6">
+    <row r="180" spans="1:12" ht="15.6">
       <c r="A180" s="1" t="s">
         <v>183</v>
       </c>
@@ -8014,17 +8551,20 @@
       <c r="H180">
         <v>2.9502000000000002</v>
       </c>
-      <c r="I180" t="s">
+      <c r="I180">
+        <v>14.901445000000001</v>
+      </c>
+      <c r="J180" t="s">
         <v>201</v>
       </c>
-      <c r="J180">
+      <c r="K180">
         <v>260588896</v>
       </c>
-      <c r="K180" t="s">
+      <c r="L180" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="15.6">
+    <row r="181" spans="1:12" ht="15.6">
       <c r="A181" s="1" t="s">
         <v>184</v>
       </c>
@@ -8047,17 +8587,20 @@
         <f t="shared" si="2"/>
         <v>0.95424250943932487</v>
       </c>
-      <c r="I181" t="s">
+      <c r="I181">
+        <v>20.238088000000001</v>
+      </c>
+      <c r="J181" t="s">
         <v>199</v>
       </c>
-      <c r="J181">
+      <c r="K181">
         <v>404962514</v>
       </c>
-      <c r="K181" t="s">
+      <c r="L181" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="15.6">
+    <row r="186" spans="1:12" ht="15.6">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>

</xml_diff>